<commit_message>
something is wrong in the scaling as the results are now very different adn the policies have no effect
</commit_message>
<xml_diff>
--- a/package/calibration_data/aligned_data.xlsx
+++ b/package/calibration_data/aligned_data.xlsx
@@ -474,7 +474,7 @@
         <v>0.6292944244731091</v>
       </c>
       <c r="C2" t="n">
-        <v>0.07846883442729451</v>
+        <v>0.07828877025570641</v>
       </c>
       <c r="D2" t="n">
         <v>0.1730509532023567</v>
@@ -491,7 +491,7 @@
         <v>0.6337245365475435</v>
       </c>
       <c r="C3" t="n">
-        <v>0.07962450100938197</v>
+        <v>0.07944178490410254</v>
       </c>
       <c r="D3" t="n">
         <v>0.1757861556172246</v>
@@ -508,7 +508,7 @@
         <v>0.6358426728695283</v>
       </c>
       <c r="C4" t="n">
-        <v>0.08200141674149457</v>
+        <v>0.08181324627506194</v>
       </c>
       <c r="D4" t="n">
         <v>0.1775596461471948</v>
@@ -525,7 +525,7 @@
         <v>0.6379608091915133</v>
       </c>
       <c r="C5" t="n">
-        <v>0.08638461674446869</v>
+        <v>0.08618638805194923</v>
       </c>
       <c r="D5" t="n">
         <v>0.1746188768886557</v>
@@ -542,7 +542,7 @@
         <v>0.6417406780855712</v>
       </c>
       <c r="C6" t="n">
-        <v>0.09316847449715111</v>
+        <v>0.09295467873605819</v>
       </c>
       <c r="D6" t="n">
         <v>0.1865239404132629</v>
@@ -559,7 +559,7 @@
         <v>0.6455205469796292</v>
       </c>
       <c r="C7" t="n">
-        <v>0.09178638894955229</v>
+        <v>0.09157576469076356</v>
       </c>
       <c r="D7" t="n">
         <v>0.1993739790347238</v>
@@ -576,7 +576,7 @@
         <v>0.6449777965743286</v>
       </c>
       <c r="C8" t="n">
-        <v>0.08451453722828758</v>
+        <v>0.08432059984863574</v>
       </c>
       <c r="D8" t="n">
         <v>0.2023325464738861</v>
@@ -593,7 +593,7 @@
         <v>0.644435046169028</v>
       </c>
       <c r="C9" t="n">
-        <v>0.07485626408242731</v>
+        <v>0.07468448975598854</v>
       </c>
       <c r="D9" t="n">
         <v>0.1986235862883644</v>
@@ -610,7 +610,7 @@
         <v>0.6447099457249594</v>
       </c>
       <c r="C10" t="n">
-        <v>0.07947760126824469</v>
+        <v>0.07929522225705347</v>
       </c>
       <c r="D10" t="n">
         <v>0.1996246542393265</v>
@@ -627,7 +627,7 @@
         <v>0.644984845280891</v>
       </c>
       <c r="C11" t="n">
-        <v>0.07404825144255989</v>
+        <v>0.07387833128061448</v>
       </c>
       <c r="D11" t="n">
         <v>0.1936479607448855</v>
@@ -644,7 +644,7 @@
         <v>0.6429213364347642</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0654667960366731</v>
+        <v>0.06531656793043313</v>
       </c>
       <c r="D12" t="n">
         <v>0.1885145089010402</v>
@@ -661,7 +661,7 @@
         <v>0.6408578275886374</v>
       </c>
       <c r="C13" t="n">
-        <v>0.05636195493766395</v>
+        <v>0.05623261991186667</v>
       </c>
       <c r="D13" t="n">
         <v>0.1913060818205316</v>
@@ -678,7 +678,7 @@
         <v>0.6448562063861281</v>
       </c>
       <c r="C14" t="n">
-        <v>0.05726858117247768</v>
+        <v>0.05713716569138751</v>
       </c>
       <c r="D14" t="n">
         <v>0.202060550413589</v>
@@ -695,7 +695,7 @@
         <v>0.6488545851836187</v>
       </c>
       <c r="C15" t="n">
-        <v>0.06098438834149893</v>
+        <v>0.06084444611543344</v>
       </c>
       <c r="D15" t="n">
         <v>0.1938801125438606</v>
@@ -712,7 +712,7 @@
         <v>0.6523384084020581</v>
       </c>
       <c r="C16" t="n">
-        <v>0.06930451958323991</v>
+        <v>0.06914548496781395</v>
       </c>
       <c r="D16" t="n">
         <v>0.1928446928460867</v>
@@ -729,7 +729,7 @@
         <v>0.6558222316204976</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0757979793962909</v>
+        <v>0.07562404409487271</v>
       </c>
       <c r="D17" t="n">
         <v>0.183738815474815</v>
@@ -746,7 +746,7 @@
         <v>0.6555755268908156</v>
       </c>
       <c r="C18" t="n">
-        <v>0.07399605081365281</v>
+        <v>0.07382625043764623</v>
       </c>
       <c r="D18" t="n">
         <v>0.1955533645497895</v>
@@ -763,7 +763,7 @@
         <v>0.6553288221611334</v>
       </c>
       <c r="C19" t="n">
-        <v>0.07475636404704668</v>
+        <v>0.0745848189634308</v>
       </c>
       <c r="D19" t="n">
         <v>0.1963899582130008</v>
@@ -780,7 +780,7 @@
         <v>0.6568196235990695</v>
       </c>
       <c r="C20" t="n">
-        <v>0.07527180708927593</v>
+        <v>0.07509907920709961</v>
       </c>
       <c r="D20" t="n">
         <v>0.2021864073919063</v>
@@ -797,7 +797,7 @@
         <v>0.6583104250370057</v>
       </c>
       <c r="C21" t="n">
-        <v>0.07460006424361178</v>
+        <v>0.07442887782461517</v>
       </c>
       <c r="D21" t="n">
         <v>0.1962599938968569</v>
@@ -814,7 +814,7 @@
         <v>0.6596021005145555</v>
       </c>
       <c r="C22" t="n">
-        <v>0.07399915791948407</v>
+        <v>0.07382935041353296</v>
       </c>
       <c r="D22" t="n">
         <v>0.1760152066062713</v>
@@ -831,7 +831,7 @@
         <v>0.6608937759921054</v>
       </c>
       <c r="C23" t="n">
-        <v>0.07167566365546442</v>
+        <v>0.07151118792324097</v>
       </c>
       <c r="D23" t="n">
         <v>0.1812696750247971</v>
@@ -848,7 +848,7 @@
         <v>0.660273489814619</v>
       </c>
       <c r="C24" t="n">
-        <v>0.07378760582024704</v>
+        <v>0.07361828376758162</v>
       </c>
       <c r="D24" t="n">
         <v>0.1900727530878695</v>
@@ -865,7 +865,7 @@
         <v>0.6596532036371325</v>
       </c>
       <c r="C25" t="n">
-        <v>0.07208333066196505</v>
+        <v>0.07191791944723643</v>
       </c>
       <c r="D25" t="n">
         <v>0.2017726879307581</v>
@@ -882,7 +882,7 @@
         <v>0.6655582575597377</v>
       </c>
       <c r="C26" t="n">
-        <v>0.07491455396077745</v>
+        <v>0.07474264587526436</v>
       </c>
       <c r="D26" t="n">
         <v>0.1924700032566304</v>
@@ -899,7 +899,7 @@
         <v>0.671463311482343</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0827893334593037</v>
+        <v>0.08259935494293497</v>
       </c>
       <c r="D27" t="n">
         <v>0.1848202245421765</v>
@@ -916,7 +916,7 @@
         <v>0.6725593853527877</v>
       </c>
       <c r="C28" t="n">
-        <v>0.09590231198121908</v>
+        <v>0.09568224282272683</v>
       </c>
       <c r="D28" t="n">
         <v>0.1697991322210112</v>
@@ -933,7 +933,7 @@
         <v>0.6736554592232326</v>
       </c>
       <c r="C29" t="n">
-        <v>0.09316335099899029</v>
+        <v>0.09294956699490202</v>
       </c>
       <c r="D29" t="n">
         <v>0.1857032378899567</v>
@@ -950,7 +950,7 @@
         <v>0.6715285120180446</v>
       </c>
       <c r="C30" t="n">
-        <v>0.08443424066925756</v>
+        <v>0.08424048754789741</v>
       </c>
       <c r="D30" t="n">
         <v>0.1897164419975911</v>
@@ -967,7 +967,7 @@
         <v>0.6694015648128568</v>
       </c>
       <c r="C31" t="n">
-        <v>0.08107241281273692</v>
+        <v>0.0808863741521869</v>
       </c>
       <c r="D31" t="n">
         <v>0.1959959565327268</v>
@@ -984,7 +984,7 @@
         <v>0.6701222950588567</v>
       </c>
       <c r="C32" t="n">
-        <v>0.08008985881492896</v>
+        <v>0.07990607484279055</v>
       </c>
       <c r="D32" t="n">
         <v>0.201455765604908</v>
@@ -1001,7 +1001,7 @@
         <v>0.6708430253048565</v>
       </c>
       <c r="C33" t="n">
-        <v>0.08554907457511361</v>
+        <v>0.08535276321970831</v>
       </c>
       <c r="D33" t="n">
         <v>0.1922953584281174</v>
@@ -1018,7 +1018,7 @@
         <v>0.671923239585536</v>
       </c>
       <c r="C34" t="n">
-        <v>0.09233197535817972</v>
+        <v>0.09212009913018031</v>
       </c>
       <c r="D34" t="n">
         <v>0.1500171359784738</v>
@@ -1035,7 +1035,7 @@
         <v>0.6730034538662155</v>
       </c>
       <c r="C35" t="n">
-        <v>0.08197580515087087</v>
+        <v>0.08178769345592227</v>
       </c>
       <c r="D35" t="n">
         <v>0.1555712669801737</v>
@@ -1052,7 +1052,7 @@
         <v>0.6714774088954677</v>
       </c>
       <c r="C36" t="n">
-        <v>0.07773902637449152</v>
+        <v>0.07756063690959947</v>
       </c>
       <c r="D36" t="n">
         <v>0.1867523737042383</v>
@@ -1069,7 +1069,7 @@
         <v>0.6699513639247199</v>
       </c>
       <c r="C37" t="n">
-        <v>0.07527412095196009</v>
+        <v>0.07510138776011185</v>
       </c>
       <c r="D37" t="n">
         <v>0.1858343854554637</v>
@@ -1086,7 +1086,7 @@
         <v>0.6752572777895257</v>
       </c>
       <c r="C38" t="n">
-        <v>0.07650417359307922</v>
+        <v>0.07632861777220316</v>
       </c>
       <c r="D38" t="n">
         <v>0.1864474536463158</v>
@@ -1103,7 +1103,7 @@
         <v>0.6805631916543314</v>
       </c>
       <c r="C39" t="n">
-        <v>0.08437129821908514</v>
+        <v>0.08417768953315889</v>
       </c>
       <c r="D39" t="n">
         <v>0.182055100127911</v>
@@ -1120,7 +1120,7 @@
         <v>0.6828381616973286</v>
       </c>
       <c r="C40" t="n">
-        <v>0.09415115265408505</v>
+        <v>0.09393510191966982</v>
       </c>
       <c r="D40" t="n">
         <v>0.1777873686764026</v>
@@ -1137,7 +1137,7 @@
         <v>0.6851131317403256</v>
       </c>
       <c r="C41" t="n">
-        <v>0.09567762893916479</v>
+        <v>0.09545807536582342</v>
       </c>
       <c r="D41" t="n">
         <v>0.1668337603012439</v>
@@ -1154,7 +1154,7 @@
         <v>0.6876700500458166</v>
       </c>
       <c r="C42" t="n">
-        <v>0.1002515668603087</v>
+        <v>0.1000215173703569</v>
       </c>
       <c r="D42" t="n">
         <v>0.174066036454583</v>
@@ -1171,7 +1171,7 @@
         <v>0.6902269683513075</v>
       </c>
       <c r="C43" t="n">
-        <v>0.1009233240572902</v>
+        <v>0.1006917330712264</v>
       </c>
       <c r="D43" t="n">
         <v>0.1796510505757104</v>
@@ -1188,7 +1188,7 @@
         <v>0.6893370691478113</v>
       </c>
       <c r="C44" t="n">
-        <v>0.09718032439894168</v>
+        <v>0.09695732255706047</v>
       </c>
       <c r="D44" t="n">
         <v>0.1768365658192415</v>
@@ -1205,7 +1205,7 @@
         <v>0.6884471699443152</v>
       </c>
       <c r="C45" t="n">
-        <v>0.09286115593324459</v>
+        <v>0.09264806538286402</v>
       </c>
       <c r="D45" t="n">
         <v>0.1815680352206409</v>
@@ -1222,7 +1222,7 @@
         <v>0.6931944738140552</v>
       </c>
       <c r="C46" t="n">
-        <v>0.09153275508803327</v>
+        <v>0.09132271284848179</v>
       </c>
       <c r="D46" t="n">
         <v>0.1757082674503145</v>
@@ -1239,7 +1239,7 @@
         <v>0.697941777683795</v>
       </c>
       <c r="C47" t="n">
-        <v>0.1021288627205429</v>
+        <v>0.101894505358219</v>
       </c>
       <c r="D47" t="n">
         <v>0.1637672419887494</v>
@@ -1256,7 +1256,7 @@
         <v>0.696169027983365</v>
       </c>
       <c r="C48" t="n">
-        <v>0.1012685097528996</v>
+        <v>0.1010361266615779</v>
       </c>
       <c r="D48" t="n">
         <v>0.1795540953065595</v>
@@ -1273,7 +1273,7 @@
         <v>0.694396278282935</v>
       </c>
       <c r="C49" t="n">
-        <v>0.09258402156038735</v>
+        <v>0.09237156695638767</v>
       </c>
       <c r="D49" t="n">
         <v>0.1785723856507705</v>
@@ -1290,7 +1290,7 @@
         <v>0.6979999295129343</v>
       </c>
       <c r="C50" t="n">
-        <v>0.08664757321996157</v>
+        <v>0.08644874111539617</v>
       </c>
       <c r="D50" t="n">
         <v>0.1746418514469794</v>
@@ -1307,7 +1307,7 @@
         <v>0.7016035807429337</v>
       </c>
       <c r="C51" t="n">
-        <v>0.0924881254615141</v>
+        <v>0.09227589091241556</v>
       </c>
       <c r="D51" t="n">
         <v>0.1757402661335289</v>
@@ -1324,7 +1324,7 @@
         <v>0.7067826178896173</v>
       </c>
       <c r="C52" t="n">
-        <v>0.09957800067317402</v>
+        <v>0.09934949683046396</v>
       </c>
       <c r="D52" t="n">
         <v>0.1595964546168518</v>
@@ -1341,7 +1341,7 @@
         <v>0.7119616550363008</v>
       </c>
       <c r="C53" t="n">
-        <v>0.1093879135892917</v>
+        <v>0.1091368987222306</v>
       </c>
       <c r="D53" t="n">
         <v>0.1702338870958161</v>
@@ -1358,7 +1358,7 @@
         <v>0.7107457531542962</v>
       </c>
       <c r="C54" t="n">
-        <v>0.1063671498063639</v>
+        <v>0.1061230667528325</v>
       </c>
       <c r="D54" t="n">
         <v>0.1768564911462956</v>
@@ -1375,7 +1375,7 @@
         <v>0.7095298512722915</v>
       </c>
       <c r="C55" t="n">
-        <v>0.1018984611716554</v>
+        <v>0.1016646325168666</v>
       </c>
       <c r="D55" t="n">
         <v>0.1888574522406891</v>
@@ -1392,7 +1392,7 @@
         <v>0.7134295481779093</v>
       </c>
       <c r="C56" t="n">
-        <v>0.1076069812304098</v>
+        <v>0.1073600531082608</v>
       </c>
       <c r="D56" t="n">
         <v>0.1844611010801345</v>
@@ -1409,7 +1409,7 @@
         <v>0.7173292450835271</v>
       </c>
       <c r="C57" t="n">
-        <v>0.1137971169577714</v>
+        <v>0.1135359841941249</v>
       </c>
       <c r="D57" t="n">
         <v>0.1872222566143415</v>
@@ -1426,7 +1426,7 @@
         <v>0.7235321068583915</v>
       </c>
       <c r="C58" t="n">
-        <v>0.1257166048856523</v>
+        <v>0.1254281202091713</v>
       </c>
       <c r="D58" t="n">
         <v>0.1677879928882827</v>
@@ -1443,7 +1443,7 @@
         <v>0.7297349686332558</v>
       </c>
       <c r="C59" t="n">
-        <v>0.1202902475187752</v>
+        <v>0.1200142148246785</v>
       </c>
       <c r="D59" t="n">
         <v>0.1548507401415083</v>
@@ -1460,7 +1460,7 @@
         <v>0.7247198139141467</v>
       </c>
       <c r="C60" t="n">
-        <v>0.1063859418767507</v>
+        <v>0.1061418157006392</v>
       </c>
       <c r="D60" t="n">
         <v>0.1766199813258637</v>
@@ -1477,7 +1477,7 @@
         <v>0.7197046591950377</v>
       </c>
       <c r="C61" t="n">
-        <v>0.09666465141105436</v>
+        <v>0.09644283289539496</v>
       </c>
       <c r="D61" t="n">
         <v>0.1793791360811717</v>
@@ -1494,7 +1494,7 @@
         <v>0.7261189821667724</v>
       </c>
       <c r="C62" t="n">
-        <v>0.1001488761290886</v>
+        <v>0.09991906228583122</v>
       </c>
       <c r="D62" t="n">
         <v>0.1809620781540462</v>
@@ -1511,7 +1511,7 @@
         <v>0.732533305138507</v>
       </c>
       <c r="C63" t="n">
-        <v>0.1040225740802217</v>
+        <v>0.1037838711765157</v>
       </c>
       <c r="D63" t="n">
         <v>0.1836093991311</v>
@@ -1528,7 +1528,7 @@
         <v>0.7371537322901247</v>
       </c>
       <c r="C64" t="n">
-        <v>0.1067891222030981</v>
+        <v>0.1065440708401657</v>
       </c>
       <c r="D64" t="n">
         <v>0.1861212851405623</v>
@@ -1545,7 +1545,7 @@
         <v>0.7417741594417424</v>
       </c>
       <c r="C65" t="n">
-        <v>0.1182974614079849</v>
+        <v>0.1180260016042951</v>
       </c>
       <c r="D65" t="n">
         <v>0.1886018786436136</v>
@@ -1562,7 +1562,7 @@
         <v>0.7426076689927398</v>
       </c>
       <c r="C66" t="n">
-        <v>0.1348087343829717</v>
+        <v>0.1344993857956417</v>
       </c>
       <c r="D66" t="n">
         <v>0.189063493231138</v>
@@ -1579,7 +1579,7 @@
         <v>0.7434411785437371</v>
       </c>
       <c r="C67" t="n">
-        <v>0.1315504209648058</v>
+        <v>0.1312485493014126</v>
       </c>
       <c r="D67" t="n">
         <v>0.2040511130916262</v>
@@ -1596,7 +1596,7 @@
         <v>0.7453055614294777</v>
       </c>
       <c r="C68" t="n">
-        <v>0.1312213474060518</v>
+        <v>0.1309202308750393</v>
       </c>
       <c r="D68" t="n">
         <v>0.2233983061667447</v>
@@ -1613,7 +1613,7 @@
         <v>0.7471699443152182</v>
       </c>
       <c r="C69" t="n">
-        <v>0.1289666437109084</v>
+        <v>0.1286707010983821</v>
       </c>
       <c r="D69" t="n">
         <v>0.1992853180630371</v>
@@ -1630,7 +1630,7 @@
         <v>0.746739973214915</v>
       </c>
       <c r="C70" t="n">
-        <v>0.117992879932037</v>
+        <v>0.1177221190582032</v>
       </c>
       <c r="D70" t="n">
         <v>0.1951147725127431</v>
@@ -1647,7 +1647,7 @@
         <v>0.746310002114612</v>
       </c>
       <c r="C71" t="n">
-        <v>0.1042328252061315</v>
+        <v>0.1039936398345122</v>
       </c>
       <c r="D71" t="n">
         <v>0.1634709432465361</v>
@@ -1664,7 +1664,7 @@
         <v>0.7450095157538592</v>
       </c>
       <c r="C72" t="n">
-        <v>0.1009919986375828</v>
+        <v>0.1007602500624392</v>
       </c>
       <c r="D72" t="n">
         <v>0.1942257071086953</v>
@@ -1681,7 +1681,7 @@
         <v>0.7437090293931063</v>
       </c>
       <c r="C73" t="n">
-        <v>0.1043553284048905</v>
+        <v>0.1041158619224689</v>
       </c>
       <c r="D73" t="n">
         <v>0.1945653397782201</v>
@@ -1698,7 +1698,7 @@
         <v>0.7505638965249877</v>
       </c>
       <c r="C74" t="n">
-        <v>0.1045613842650201</v>
+        <v>0.1043214449416543</v>
       </c>
       <c r="D74" t="n">
         <v>0.199583274246942</v>
@@ -1715,7 +1715,7 @@
         <v>0.7574187636568689</v>
       </c>
       <c r="C75" t="n">
-        <v>0.1074570685403192</v>
+        <v>0.1072104844261391</v>
       </c>
       <c r="D75" t="n">
         <v>0.1872147968917222</v>
@@ -1732,7 +1732,7 @@
         <v>0.7623422851906676</v>
       </c>
       <c r="C76" t="n">
-        <v>0.1221892079313198</v>
+        <v>0.1219088176507232</v>
       </c>
       <c r="D76" t="n">
         <v>0.1812833981332088</v>
@@ -1749,7 +1749,7 @@
         <v>0.7672658067244661</v>
       </c>
       <c r="C77" t="n">
-        <v>0.1305544950942564</v>
+        <v>0.1302549088040072</v>
       </c>
       <c r="D77" t="n">
         <v>0.1790774446036821</v>
@@ -1766,7 +1766,7 @@
         <v>0.7667371537322901</v>
       </c>
       <c r="C78" t="n">
-        <v>0.1363570285997959</v>
+        <v>0.1360441271074488</v>
       </c>
       <c r="D78" t="n">
         <v>0.1845482500896329</v>
@@ -1783,7 +1783,7 @@
         <v>0.7662085007401142</v>
       </c>
       <c r="C79" t="n">
-        <v>0.1303431114422918</v>
+        <v>0.1300440102187886</v>
       </c>
       <c r="D79" t="n">
         <v>0.1921148092951372</v>
@@ -1800,7 +1800,7 @@
         <v>0.7663424261647988</v>
       </c>
       <c r="C80" t="n">
-        <v>0.1242525491855299</v>
+        <v>0.1239674241100768</v>
       </c>
       <c r="D80" t="n">
         <v>0.197431324215193</v>
@@ -1817,7 +1817,7 @@
         <v>0.7664763515894832</v>
       </c>
       <c r="C81" t="n">
-        <v>0.115385164612838</v>
+        <v>0.1151203877210795</v>
       </c>
       <c r="D81" t="n">
         <v>0.1971358929556741</v>
@@ -1834,7 +1834,7 @@
         <v>0.7690826108409106</v>
       </c>
       <c r="C82" t="n">
-        <v>0.1139799532122473</v>
+        <v>0.1137184008901999</v>
       </c>
       <c r="D82" t="n">
         <v>0.1963378158230589</v>
@@ -1851,7 +1851,7 @@
         <v>0.771688870092338</v>
       </c>
       <c r="C83" t="n">
-        <v>0.1209814001708082</v>
+        <v>0.1207037814734194</v>
       </c>
       <c r="D83" t="n">
         <v>0.1623711379756027</v>
@@ -1868,7 +1868,7 @@
         <v>0.7728060900824699</v>
       </c>
       <c r="C84" t="n">
-        <v>0.1317536200952225</v>
+        <v>0.131451282146286</v>
       </c>
       <c r="D84" t="n">
         <v>0.1859457396158266</v>
@@ -1885,7 +1885,7 @@
         <v>0.7739233100726016</v>
       </c>
       <c r="C85" t="n">
-        <v>0.1299741184828296</v>
+        <v>0.1296758639956397</v>
       </c>
       <c r="D85" t="n">
         <v>0.1868402180397372</v>
@@ -1902,7 +1902,7 @@
         <v>0.7770317896665961</v>
       </c>
       <c r="C86" t="n">
-        <v>0.1272534808935253</v>
+        <v>0.126961469513644</v>
       </c>
       <c r="D86" t="n">
         <v>0.1766980473976641</v>
@@ -1919,7 +1919,7 @@
         <v>0.7801402692605907</v>
       </c>
       <c r="C87" t="n">
-        <v>0.1242468871551385</v>
+        <v>0.1239617750724718</v>
       </c>
       <c r="D87" t="n">
         <v>0.1712512547604096</v>
@@ -1936,7 +1936,7 @@
         <v>0.7853668851765701</v>
       </c>
       <c r="C88" t="n">
-        <v>0.1378591357027464</v>
+        <v>0.1375427872919748</v>
       </c>
       <c r="D88" t="n">
         <v>0.1674376682821756</v>
@@ -1953,7 +1953,7 @@
         <v>0.7905935010925496</v>
       </c>
       <c r="C89" t="n">
-        <v>0.1459409922299541</v>
+        <v>0.1456060982040847</v>
       </c>
       <c r="D89" t="n">
         <v>0.1635480178135991</v>
@@ -1970,7 +1970,7 @@
         <v>0.797643969831536</v>
       </c>
       <c r="C90" t="n">
-        <v>0.1510072219632517</v>
+        <v>0.1506607023478516</v>
       </c>
       <c r="D90" t="n">
         <v>0.1698752891325912</v>
@@ -1987,7 +1987,7 @@
         <v>0.8046944385705224</v>
       </c>
       <c r="C91" t="n">
-        <v>0.168921261890997</v>
+        <v>0.1685336345315744</v>
       </c>
       <c r="D91" t="n">
         <v>0.1801926210122457</v>
@@ -2004,7 +2004,7 @@
         <v>0.8041657855783464</v>
       </c>
       <c r="C92" t="n">
-        <v>0.1682861947461148</v>
+        <v>0.1679000246893294</v>
       </c>
       <c r="D92" t="n">
         <v>0.1790675537090115</v>
@@ -2021,7 +2021,7 @@
         <v>0.8036371325861704</v>
       </c>
       <c r="C93" t="n">
-        <v>0.1540994000631512</v>
+        <v>0.1537457847582074</v>
       </c>
       <c r="D93" t="n">
         <v>0.1811762972318703</v>
@@ -2038,7 +2038,7 @@
         <v>0.8010784521040389</v>
       </c>
       <c r="C94" t="n">
-        <v>0.1438810389884645</v>
+        <v>0.1435508719829038</v>
       </c>
       <c r="D94" t="n">
         <v>0.1750140696354565</v>
@@ -2055,7 +2055,7 @@
         <v>0.7985197716219073</v>
       </c>
       <c r="C95" t="n">
-        <v>0.1292391292834066</v>
+        <v>0.1289425613922046</v>
       </c>
       <c r="D95" t="n">
         <v>0.1639283141782744</v>
@@ -2072,7 +2072,7 @@
         <v>0.7865422569958412</v>
       </c>
       <c r="C96" t="n">
-        <v>0.09562105447107296</v>
+        <v>0.09540163072041601</v>
       </c>
       <c r="D96" t="n">
         <v>0.1807913036269987</v>
@@ -2089,7 +2089,7 @@
         <v>0.7745647423697751</v>
       </c>
       <c r="C97" t="n">
-        <v>0.07246650528950062</v>
+        <v>0.07230021479547105</v>
       </c>
       <c r="D97" t="n">
         <v>0.1768735297463315</v>
@@ -2106,7 +2106,7 @@
         <v>0.7788045393670262</v>
       </c>
       <c r="C98" t="n">
-        <v>0.07900570283014599</v>
+        <v>0.07882440669474808</v>
       </c>
       <c r="D98" t="n">
         <v>0.1887508258740689</v>
@@ -2123,7 +2123,7 @@
         <v>0.7830443363642772</v>
       </c>
       <c r="C99" t="n">
-        <v>0.08677669557702954</v>
+        <v>0.08657756717253273</v>
       </c>
       <c r="D99" t="n">
         <v>0.1805772590815596</v>
@@ -2140,7 +2140,7 @@
         <v>0.7843042926622964</v>
       </c>
       <c r="C100" t="n">
-        <v>0.08564278001334601</v>
+        <v>0.08544625362999703</v>
       </c>
       <c r="D100" t="n">
         <v>0.1802871682877345</v>
@@ -2157,7 +2157,7 @@
         <v>0.7855642489603157</v>
       </c>
       <c r="C101" t="n">
-        <v>0.090775515935683</v>
+        <v>0.09056721134957899</v>
       </c>
       <c r="D101" t="n">
         <v>0.1777066614026273</v>
@@ -2174,7 +2174,7 @@
         <v>0.7892612955522661</v>
       </c>
       <c r="C102" t="n">
-        <v>0.09620388131014312</v>
+        <v>0.09598312013383532</v>
       </c>
       <c r="D102" t="n">
         <v>0.190177829377749</v>
@@ -2191,7 +2191,7 @@
         <v>0.7929583421442165</v>
       </c>
       <c r="C103" t="n">
-        <v>0.1123262033654231</v>
+        <v>0.1120684459397616</v>
       </c>
       <c r="D103" t="n">
         <v>0.1862645137203659</v>
@@ -2208,7 +2208,7 @@
         <v>0.7937407485726369</v>
       </c>
       <c r="C104" t="n">
-        <v>0.1103634910485933</v>
+        <v>0.110110237502338</v>
       </c>
       <c r="D104" t="n">
         <v>0.1972936381074169</v>
@@ -2225,7 +2225,7 @@
         <v>0.7945231550010572</v>
       </c>
       <c r="C105" t="n">
-        <v>0.1154277246959253</v>
+        <v>0.1151628501406019</v>
       </c>
       <c r="D105" t="n">
         <v>0.2004976179703511</v>
@@ -2242,7 +2242,7 @@
         <v>0.7955751744554873</v>
       </c>
       <c r="C106" t="n">
-        <v>0.1194984497411805</v>
+        <v>0.1192242340029737</v>
       </c>
       <c r="D106" t="n">
         <v>0.1952046833365451</v>
@@ -2259,7 +2259,7 @@
         <v>0.7966271939099175</v>
       </c>
       <c r="C107" t="n">
-        <v>0.1153111526975911</v>
+        <v>0.1150465456426131</v>
       </c>
       <c r="D107" t="n">
         <v>0.1738579865949963</v>
@@ -2276,7 +2276,7 @@
         <v>0.7936561640938887</v>
       </c>
       <c r="C108" t="n">
-        <v>0.1136260311201108</v>
+        <v>0.1133652909509237</v>
       </c>
       <c r="D108" t="n">
         <v>0.1708548438665672</v>
@@ -2293,7 +2293,7 @@
         <v>0.7906851342778599</v>
       </c>
       <c r="C109" t="n">
-        <v>0.1124594306192584</v>
+        <v>0.112201367474068</v>
       </c>
       <c r="D109" t="n">
         <v>0.1862941310190819</v>
@@ -2310,7 +2310,7 @@
         <v>0.7929354338478889</v>
       </c>
       <c r="C110" t="n">
-        <v>0.1159615223067948</v>
+        <v>0.115695422834276</v>
       </c>
       <c r="D110" t="n">
         <v>0.1914405555864215</v>
@@ -2327,7 +2327,7 @@
         <v>0.7951857334179178</v>
       </c>
       <c r="C111" t="n">
-        <v>0.1129170157694592</v>
+        <v>0.1126579025934942</v>
       </c>
       <c r="D111" t="n">
         <v>0.1787003891395495</v>
@@ -2344,7 +2344,7 @@
         <v>0.7976192993585678</v>
       </c>
       <c r="C112" t="n">
-        <v>0.116747425839477</v>
+        <v>0.1164795229367226</v>
       </c>
       <c r="D112" t="n">
         <v>0.1853014340536372</v>
@@ -2361,7 +2361,7 @@
         <v>0.8000528652992176</v>
       </c>
       <c r="C113" t="n">
-        <v>0.1176672243587202</v>
+        <v>0.1173972107739402</v>
       </c>
       <c r="D113" t="n">
         <v>0.1738635108168471</v>
@@ -2378,7 +2378,7 @@
         <v>0.8002396560231197</v>
       </c>
       <c r="C114" t="n">
-        <v>0.1175647811151238</v>
+        <v>0.1172950026091228</v>
       </c>
       <c r="D114" t="n">
         <v>0.1861942217915969</v>
@@ -2395,7 +2395,7 @@
         <v>0.8004264467470219</v>
       </c>
       <c r="C115" t="n">
-        <v>0.1174623856846592</v>
+        <v>0.1171928421477194</v>
       </c>
       <c r="D115" t="n">
         <v>0.187400104793649</v>
@@ -2412,7 +2412,7 @@
         <v>0.8009339536195108</v>
       </c>
       <c r="C116" t="n">
-        <v>0.1187738384296193</v>
+        <v>0.1185012854730314</v>
       </c>
       <c r="D116" t="n">
         <v>0.1876559225898432</v>
@@ -2429,7 +2429,7 @@
         <v>0.8014414604919997</v>
       </c>
       <c r="C117" t="n">
-        <v>0.119260114071618</v>
+        <v>0.1189864452475486</v>
       </c>
       <c r="D117" t="n">
         <v>0.1895334936961579</v>
@@ -2446,7 +2446,7 @@
         <v>0.8020335518432368</v>
       </c>
       <c r="C118" t="n">
-        <v>0.1146086716556297</v>
+        <v>0.114345676599451</v>
       </c>
       <c r="D118" t="n">
         <v>0.1851543487909162</v>
@@ -2463,7 +2463,7 @@
         <v>0.8026256431944737</v>
       </c>
       <c r="C119" t="n">
-        <v>0.1175890663352903</v>
+        <v>0.1173192321014569</v>
       </c>
       <c r="D119" t="n">
         <v>0.1757980214018803</v>
@@ -2480,7 +2480,7 @@
         <v>0.8021850990343271</v>
       </c>
       <c r="C120" t="n">
-        <v>0.1198601172170184</v>
+        <v>0.1195850715524478</v>
       </c>
       <c r="D120" t="n">
         <v>0.1828754986556069</v>
@@ -2497,7 +2497,7 @@
         <v>0.8017445548741805</v>
       </c>
       <c r="C121" t="n">
-        <v>0.1233684711653853</v>
+        <v>0.1230853748033376</v>
       </c>
       <c r="D121" t="n">
         <v>0.1865930976275568</v>
@@ -2514,7 +2514,7 @@
         <v>0.8067685204764925</v>
       </c>
       <c r="C122" t="n">
-        <v>0.1260212779992355</v>
+        <v>0.1257320941826155</v>
       </c>
       <c r="D122" t="n">
         <v>0.1889017681428494</v>
@@ -2531,7 +2531,7 @@
         <v>0.8117924860788045</v>
       </c>
       <c r="C123" t="n">
-        <v>0.1321519992359055</v>
+        <v>0.1318487471175352</v>
       </c>
       <c r="D123" t="n">
         <v>0.1771388654933185</v>
@@ -2548,7 +2548,7 @@
         <v>0.8184447028970184</v>
       </c>
       <c r="C124" t="n">
-        <v>0.1466928670624027</v>
+        <v>0.1463562476927095</v>
       </c>
       <c r="D124" t="n">
         <v>0.1743550902032722</v>
@@ -2565,7 +2565,7 @@
         <v>0.8250969197152322</v>
       </c>
       <c r="C125" t="n">
-        <v>0.1529274888622161</v>
+        <v>0.1525765627678501</v>
       </c>
       <c r="D125" t="n">
         <v>0.1711314108998646</v>
@@ -2582,7 +2582,7 @@
         <v>0.8236378374568267</v>
       </c>
       <c r="C126" t="n">
-        <v>0.1540361482077373</v>
+        <v>0.1536826780482264</v>
       </c>
       <c r="D126" t="n">
         <v>0.177505201134793</v>
@@ -2599,7 +2599,7 @@
         <v>0.8221787551984211</v>
       </c>
       <c r="C127" t="n">
-        <v>0.1446765672889384</v>
+        <v>0.1443445747669744</v>
       </c>
       <c r="D127" t="n">
         <v>0.1801311443084639</v>
@@ -2616,7 +2616,7 @@
         <v>0.822127652075844</v>
       </c>
       <c r="C128" t="n">
-        <v>0.1402701876148077</v>
+        <v>0.1399483065098351</v>
       </c>
       <c r="D128" t="n">
         <v>0.1909679106445093</v>
@@ -2633,7 +2633,7 @@
         <v>0.8220765489532671</v>
       </c>
       <c r="C129" t="n">
-        <v>0.1395125553040436</v>
+        <v>0.1391924127547078</v>
       </c>
       <c r="D129" t="n">
         <v>0.1842894073464348</v>
@@ -2650,7 +2650,7 @@
         <v>0.8239462183689292</v>
       </c>
       <c r="C130" t="n">
-        <v>0.1445846796115259</v>
+        <v>0.1442528979462496</v>
       </c>
       <c r="D130" t="n">
         <v>0.1796233743180209</v>
@@ -2667,7 +2667,7 @@
         <v>0.8258158877845915</v>
       </c>
       <c r="C131" t="n">
-        <v>0.1413147915004033</v>
+        <v>0.1409905133197679</v>
       </c>
       <c r="D131" t="n">
         <v>0.1714667907151423</v>
@@ -2684,7 +2684,7 @@
         <v>0.8234686684993304</v>
       </c>
       <c r="C132" t="n">
-        <v>0.1401874830409457</v>
+        <v>0.1398657917199897</v>
       </c>
       <c r="D132" t="n">
         <v>0.180577605060539</v>
@@ -2701,7 +2701,7 @@
         <v>0.8211214492140693</v>
       </c>
       <c r="C133" t="n">
-        <v>0.1332811365538554</v>
+        <v>0.1329752933790835</v>
       </c>
       <c r="D133" t="n">
         <v>0.1799977337596841</v>
@@ -2718,7 +2718,7 @@
         <v>0.8261313174032564</v>
       </c>
       <c r="C134" t="n">
-        <v>0.1360679563066724</v>
+        <v>0.1357557181549161</v>
       </c>
       <c r="D134" t="n">
         <v>0.185079534910508</v>
@@ -2735,7 +2735,7 @@
         <v>0.8311411855924438</v>
       </c>
       <c r="C135" t="n">
-        <v>0.145354365893787</v>
+        <v>0.1450208180123586</v>
       </c>
       <c r="D135" t="n">
         <v>0.1751808267042082</v>
@@ -2752,7 +2752,7 @@
         <v>0.8351272291534503</v>
       </c>
       <c r="C136" t="n">
-        <v>0.1585626661152351</v>
+        <v>0.1581988088548689</v>
       </c>
       <c r="D136" t="n">
         <v>0.1760210838161876</v>
@@ -2769,7 +2769,7 @@
         <v>0.8391132727144569</v>
       </c>
       <c r="C137" t="n">
-        <v>0.1534476979293544</v>
+        <v>0.1530955780997251</v>
       </c>
       <c r="D137" t="n">
         <v>0.1747082363812004</v>
@@ -2786,7 +2786,7 @@
         <v>0.8385687601325156</v>
       </c>
       <c r="C138" t="n">
-        <v>0.1557296267265709</v>
+        <v>0.1553722705044107</v>
       </c>
       <c r="D138" t="n">
         <v>0.17911470965871</v>
@@ -2803,7 +2803,7 @@
         <v>0.8380242475505745</v>
       </c>
       <c r="C139" t="n">
-        <v>0.1479551461218516</v>
+        <v>0.147615630172455</v>
       </c>
       <c r="D139" t="n">
         <v>0.18997063684651</v>
@@ -2820,7 +2820,7 @@
         <v>0.8402322548812292</v>
       </c>
       <c r="C140" t="n">
-        <v>0.1364265646005264</v>
+        <v>0.136113503542379</v>
       </c>
       <c r="D140" t="n">
         <v>0.1811403919759236</v>
@@ -2837,7 +2837,7 @@
         <v>0.8424402622118841</v>
       </c>
       <c r="C141" t="n">
-        <v>0.1463249152840182</v>
+        <v>0.1459891402614169</v>
       </c>
       <c r="D141" t="n">
         <v>0.1953847737141997</v>
@@ -2854,7 +2854,7 @@
         <v>0.846850990343272</v>
       </c>
       <c r="C142" t="n">
-        <v>0.1491761849965978</v>
+        <v>0.1488338671022626</v>
       </c>
       <c r="D142" t="n">
         <v>0.1986181771267929</v>
@@ -2871,7 +2871,7 @@
         <v>0.8512617184746599</v>
       </c>
       <c r="C143" t="n">
-        <v>0.1571079693794325</v>
+        <v>0.1567474502438717</v>
       </c>
       <c r="D143" t="n">
         <v>0.1670461585595581</v>
@@ -2888,7 +2888,7 @@
         <v>0.8445090575879326</v>
       </c>
       <c r="C144" t="n">
-        <v>0.1382933657734506</v>
+        <v>0.1379760209253223</v>
       </c>
       <c r="D144" t="n">
         <v>0.1761970444994387</v>
@@ -2905,7 +2905,7 @@
         <v>0.8377563967012054</v>
       </c>
       <c r="C145" t="n">
-        <v>0.1299184350350224</v>
+        <v>0.1296203083258729</v>
       </c>
       <c r="D145" t="n">
         <v>0.1848986180349593</v>
@@ -2922,7 +2922,7 @@
         <v>0.8439892154789596</v>
       </c>
       <c r="C146" t="n">
-        <v>0.1307362676872389</v>
+        <v>0.1304362642793963</v>
       </c>
       <c r="D146" t="n">
         <v>0.1914716409122512</v>
@@ -2939,7 +2939,7 @@
         <v>0.8502220342567138</v>
       </c>
       <c r="C147" t="n">
-        <v>0.1456207849379461</v>
+        <v>0.1452866256988388</v>
       </c>
       <c r="D147" t="n">
         <v>0.1800706095953441</v>
@@ -2956,7 +2956,7 @@
         <v>0.8504986959892858</v>
       </c>
       <c r="C148" t="n">
-        <v>0.1478661879119263</v>
+        <v>0.1475268760969034</v>
       </c>
       <c r="D148" t="n">
         <v>0.1793065653353114</v>
@@ -2973,7 +2973,7 @@
         <v>0.850775357721858</v>
       </c>
       <c r="C149" t="n">
-        <v>0.1421409293327644</v>
+        <v>0.1418147553953551</v>
       </c>
       <c r="D149" t="n">
         <v>0.1796008765570694</v>
@@ -2990,7 +2990,7 @@
         <v>0.851704024811447</v>
       </c>
       <c r="C150" t="n">
-        <v>0.1426904141105881</v>
+        <v>0.1423629792582941</v>
       </c>
       <c r="D150" t="n">
         <v>0.1869193937826515</v>
@@ -3007,7 +3007,7 @@
         <v>0.8526326919010361</v>
       </c>
       <c r="C151" t="n">
-        <v>0.1424998139927085</v>
+        <v>0.1421728165147247</v>
       </c>
       <c r="D151" t="n">
         <v>0.2009071451600903</v>
@@ -3024,7 +3024,7 @@
         <v>0.8527049411433002</v>
       </c>
       <c r="C152" t="n">
-        <v>0.1426988330064704</v>
+        <v>0.1423713788351496</v>
       </c>
       <c r="D152" t="n">
         <v>0.1973719065991862</v>
@@ -3041,7 +3041,7 @@
         <v>0.8527771903855643</v>
       </c>
       <c r="C153" t="n">
-        <v>0.1378671959399422</v>
+        <v>0.137550829033166</v>
       </c>
       <c r="D153" t="n">
         <v>0.1913747246525353</v>
@@ -3058,7 +3058,7 @@
         <v>0.8539508000281948</v>
       </c>
       <c r="C154" t="n">
-        <v>0.1401368790755262</v>
+        <v>0.13981530387661</v>
       </c>
       <c r="D154" t="n">
         <v>0.1989575980189847</v>
@@ -3075,7 +3075,7 @@
         <v>0.8551244096708254</v>
       </c>
       <c r="C155" t="n">
-        <v>0.1343313308577151</v>
+        <v>0.1340230777788239</v>
       </c>
       <c r="D155" t="n">
         <v>0.1893291761631765</v>
@@ -3092,7 +3092,7 @@
         <v>0.8531736801296962</v>
       </c>
       <c r="C156" t="n">
-        <v>0.128027859442869</v>
+        <v>0.1277340710793864</v>
       </c>
       <c r="D156" t="n">
         <v>0.1937471863582005</v>
@@ -3109,7 +3109,7 @@
         <v>0.851222950588567</v>
       </c>
       <c r="C157" t="n">
-        <v>0.1283565015774699</v>
+        <v>0.1280619590716052</v>
       </c>
       <c r="D157" t="n">
         <v>0.1905493735664069</v>
@@ -3126,7 +3126,7 @@
         <v>0.8556477761330795</v>
       </c>
       <c r="C158" t="n">
-        <v>0.1285341972102487</v>
+        <v>0.1282392469422815</v>
       </c>
       <c r="D158" t="n">
         <v>0.1936544506068213</v>
@@ -3143,7 +3143,7 @@
         <v>0.8600726016775921</v>
       </c>
       <c r="C159" t="n">
-        <v>0.129965772403365</v>
+        <v>0.1296675370681084</v>
       </c>
       <c r="D159" t="n">
         <v>0.187309768600663</v>
@@ -3160,7 +3160,7 @@
         <v>0.8633555367590047</v>
       </c>
       <c r="C160" t="n">
-        <v>0.1384365940927099</v>
+        <v>0.1381189205753865</v>
       </c>
       <c r="D160" t="n">
         <v>0.1837018392160625</v>
@@ -3177,7 +3177,7 @@
         <v>0.8666384718404173</v>
       </c>
       <c r="C161" t="n">
-        <v>0.1457355103700691</v>
+        <v>0.1454010878679728</v>
       </c>
       <c r="D161" t="n">
         <v>0.1167730296868646</v>
@@ -3194,7 +3194,7 @@
         <v>0.8689786424191162</v>
       </c>
       <c r="C162" t="n">
-        <v>0.1456882756606804</v>
+        <v>0.1453539615491174</v>
       </c>
       <c r="D162" t="n">
         <v>0.1894177738842653</v>
@@ -3211,7 +3211,7 @@
         <v>0.8713188129978149</v>
       </c>
       <c r="C163" t="n">
-        <v>0.1433344467455143</v>
+        <v>0.1430055340172746</v>
       </c>
       <c r="D163" t="n">
         <v>0.1939588557930332</v>
@@ -3228,7 +3228,7 @@
         <v>0.871373440473673</v>
       </c>
       <c r="C164" t="n">
-        <v>0.1415007553282493</v>
+        <v>0.141176050412301</v>
       </c>
       <c r="D164" t="n">
         <v>0.2023242754612356</v>
@@ -3245,7 +3245,7 @@
         <v>0.8714280679495312</v>
       </c>
       <c r="C165" t="n">
-        <v>0.1363623738670786</v>
+        <v>0.1360494601088284</v>
       </c>
       <c r="D165" t="n">
         <v>0.2073607755430541</v>
@@ -3262,7 +3262,7 @@
         <v>0.8718192711637415</v>
       </c>
       <c r="C166" t="n">
-        <v>0.1314836730403848</v>
+        <v>0.1311819545449315</v>
       </c>
       <c r="D166" t="n">
         <v>0.2061207017827546</v>
@@ -3279,7 +3279,7 @@
         <v>0.8722104743779516</v>
       </c>
       <c r="C167" t="n">
-        <v>0.1233073932948388</v>
+        <v>0.1230244370895329</v>
       </c>
       <c r="D167" t="n">
         <v>0.153059386377136</v>
@@ -3296,7 +3296,7 @@
         <v>0.8675072249242264</v>
       </c>
       <c r="C168" t="n">
-        <v>0.1118376852809201</v>
+        <v>0.1115810488685225</v>
       </c>
       <c r="D168" t="n">
         <v>0.1959637857942323</v>
@@ -3313,7 +3313,7 @@
         <v>0.8628039754705011</v>
       </c>
       <c r="C169" t="n">
-        <v>0.1013903534140483</v>
+        <v>0.10115769072538</v>
       </c>
       <c r="D169" t="n">
         <v>0.1973797117788344</v>
@@ -3330,7 +3330,7 @@
         <v>0.8652815958271657</v>
       </c>
       <c r="C170" t="n">
-        <v>0.09000538134126225</v>
+        <v>0.08979884400006212</v>
       </c>
       <c r="D170" t="n">
         <v>0.2010906054619881</v>
@@ -3347,7 +3347,7 @@
         <v>0.8677592161838302</v>
       </c>
       <c r="C171" t="n">
-        <v>0.095279886929469</v>
+        <v>0.09506124606352291</v>
       </c>
       <c r="D171" t="n">
         <v>0.197404990699299</v>
@@ -3364,7 +3364,7 @@
         <v>0.8720219214774089</v>
       </c>
       <c r="C172" t="n">
-        <v>0.1165567028725586</v>
+        <v>0.1162892376260188</v>
       </c>
       <c r="D172" t="n">
         <v>0.1950639035677117</v>
@@ -3381,7 +3381,7 @@
         <v>0.8762846267709875</v>
       </c>
       <c r="C173" t="n">
-        <v>0.1116418079368718</v>
+        <v>0.1113856210085522</v>
       </c>
       <c r="D173" t="n">
         <v>0.1420771244826796</v>
@@ -3398,7 +3398,7 @@
         <v>0.8793983928949037</v>
       </c>
       <c r="C174" t="n">
-        <v>0.1297705350862955</v>
+        <v>0.1294727477664327</v>
       </c>
       <c r="D174" t="n">
         <v>0.1968391134195387</v>
@@ -3415,7 +3415,7 @@
         <v>0.88251215901882</v>
       </c>
       <c r="C175" t="n">
-        <v>0.1222419418220156</v>
+        <v>0.1219614305317925</v>
       </c>
       <c r="D175" t="n">
         <v>0.1947848516796856</v>
@@ -3432,7 +3432,7 @@
         <v>0.8840082469866779</v>
       </c>
       <c r="C176" t="n">
-        <v>0.1293653089660864</v>
+        <v>0.129068451527573</v>
       </c>
       <c r="D176" t="n">
         <v>0.2031655254486631</v>
@@ -3449,7 +3449,7 @@
         <v>0.8855043349545357</v>
       </c>
       <c r="C177" t="n">
-        <v>0.1217611204642333</v>
+        <v>0.1214817125254248</v>
       </c>
       <c r="D177" t="n">
         <v>0.205532590655634</v>
@@ -3466,7 +3466,7 @@
         <v>0.8855078593078169</v>
       </c>
       <c r="C178" t="n">
-        <v>0.1075653919937593</v>
+        <v>0.1073185593073524</v>
       </c>
       <c r="D178" t="n">
         <v>0.2072257158094996</v>
@@ -3483,7 +3483,7 @@
         <v>0.8855113836610982</v>
       </c>
       <c r="C179" t="n">
-        <v>0.09977285626156693</v>
+        <v>0.09954390527942426</v>
       </c>
       <c r="D179" t="n">
         <v>0.1689419275238304</v>
@@ -3500,7 +3500,7 @@
         <v>0.8845527595686191</v>
       </c>
       <c r="C180" t="n">
-        <v>0.09560763796751173</v>
+        <v>0.09538824500400254</v>
       </c>
       <c r="D180" t="n">
         <v>0.1959182175685206</v>
@@ -3517,7 +3517,7 @@
         <v>0.8835941354761402</v>
       </c>
       <c r="C181" t="n">
-        <v>0.09425141776786816</v>
+        <v>0.09403513695287656</v>
       </c>
       <c r="D181" t="n">
         <v>0.1956780755531269</v>
@@ -3534,7 +3534,7 @@
         <v>0.8870092338055967</v>
       </c>
       <c r="C182" t="n">
-        <v>0.0954781492371265</v>
+        <v>0.09525905341427368</v>
       </c>
       <c r="D182" t="n">
         <v>0.2003361331849968</v>
@@ -3551,7 +3551,7 @@
         <v>0.8904243321350532</v>
       </c>
       <c r="C183" t="n">
-        <v>0.08345459273537595</v>
+        <v>0.08326308763381818</v>
       </c>
       <c r="D183" t="n">
         <v>0.1985570178389782</v>
@@ -3568,7 +3568,7 @@
         <v>0.8930411644463241</v>
       </c>
       <c r="C184" t="n">
-        <v>0.08999585147883807</v>
+        <v>0.08978933600602422</v>
       </c>
       <c r="D184" t="n">
         <v>0.1976392657212258</v>
@@ -3585,7 +3585,7 @@
         <v>0.8956579967575949</v>
       </c>
       <c r="C185" t="n">
-        <v>0.09452268645675116</v>
+        <v>0.09430578315549354</v>
       </c>
       <c r="D185" t="n">
         <v>0.1383340521142389</v>
@@ -3602,7 +3602,7 @@
         <v>0.8981990554733206</v>
       </c>
       <c r="C186" t="n">
-        <v>0.0953574817052834</v>
+        <v>0.09513866278088737</v>
       </c>
       <c r="D186" t="n">
         <v>0.1971723293637559</v>
@@ -3619,7 +3619,7 @@
         <v>0.9007401141890462</v>
       </c>
       <c r="C187" t="n">
-        <v>0.09758641656493569</v>
+        <v>0.09736248285437066</v>
       </c>
       <c r="D187" t="n">
         <v>0.2008348436472908</v>
@@ -3636,7 +3636,7 @@
         <v>0.9016582082187918</v>
       </c>
       <c r="C188" t="n">
-        <v>0.09685488270829221</v>
+        <v>0.09663262766466349</v>
       </c>
       <c r="D188" t="n">
         <v>0.2048448051783072</v>
@@ -3653,7 +3653,7 @@
         <v>0.9025763022485372</v>
       </c>
       <c r="C189" t="n">
-        <v>0.09123882357075641</v>
+        <v>0.09102945582236499</v>
       </c>
       <c r="D189" t="n">
         <v>0.2090681968160502</v>
@@ -3670,7 +3670,7 @@
         <v>0.9056407274265172</v>
       </c>
       <c r="C190" t="n">
-        <v>0.09285138957801892</v>
+        <v>0.0926383214387099</v>
       </c>
       <c r="D190" t="n">
         <v>0.2011835317054947</v>
@@ -3687,7 +3687,7 @@
         <v>0.9087051526044971</v>
       </c>
       <c r="C191" t="n">
-        <v>0.09448609348578166</v>
+        <v>0.09426927415522465</v>
       </c>
       <c r="D191" t="n">
         <v>0.1532950480150173</v>
@@ -3704,7 +3704,7 @@
         <v>0.9071491506308592</v>
       </c>
       <c r="C192" t="n">
-        <v>0.09220093514041675</v>
+        <v>0.09198935961330616</v>
       </c>
       <c r="D192" t="n">
         <v>0.1976521720549584</v>
@@ -3721,7 +3721,7 @@
         <v>0.9055931486572213</v>
       </c>
       <c r="C193" t="n">
-        <v>0.09070298303580811</v>
+        <v>0.09049484489255526</v>
       </c>
       <c r="D193" t="n">
         <v>0.2005315524629018</v>
@@ -3738,7 +3738,7 @@
         <v>0.9111581024881933</v>
       </c>
       <c r="C194" t="n">
-        <v>0.09377077344390637</v>
+        <v>0.09355559557408598</v>
       </c>
       <c r="D194" t="n">
         <v>0.201611552921882</v>
@@ -3755,7 +3755,7 @@
         <v>0.9167230563191654</v>
       </c>
       <c r="C195" t="n">
-        <v>0.09640861478368851</v>
+        <v>0.09618738380094635</v>
       </c>
       <c r="D195" t="n">
         <v>0.2072599774711565</v>
@@ -3772,7 +3772,7 @@
         <v>0.9197874814971453</v>
       </c>
       <c r="C196" t="n">
-        <v>0.09977304741158821</v>
+        <v>0.09954409599080938</v>
       </c>
       <c r="D196" t="n">
         <v>0.2085264301355848</v>
@@ -3789,7 +3789,7 @@
         <v>0.9228519066751252</v>
       </c>
       <c r="C197" t="n">
-        <v>0.09970180408630895</v>
+        <v>0.09947301614916589</v>
       </c>
       <c r="D197" t="n">
         <v>0.1530039641015849</v>
@@ -3806,7 +3806,7 @@
         <v>0.9236202156904207</v>
       </c>
       <c r="C198" t="n">
-        <v>0.1007232176381703</v>
+        <v>0.1004920858407366</v>
       </c>
       <c r="D198" t="n">
         <v>0.195534914602317</v>
@@ -3823,7 +3823,7 @@
         <v>0.9243885247057165</v>
       </c>
       <c r="C199" t="n">
-        <v>0.09995796954469548</v>
+        <v>0.0997285937790038</v>
       </c>
       <c r="D199" t="n">
         <v>0.2068394348154305</v>
@@ -3840,7 +3840,7 @@
         <v>0.9264802283780926</v>
       </c>
       <c r="C200" t="n">
-        <v>0.09730374943652889</v>
+        <v>0.0970804643684814</v>
       </c>
       <c r="D200" t="n">
         <v>0.1998963327303955</v>
@@ -3857,7 +3857,7 @@
         <v>0.9285719320504687</v>
       </c>
       <c r="C201" t="n">
-        <v>0.09928148463030366</v>
+        <v>0.09905366120952178</v>
       </c>
       <c r="D201" t="n">
         <v>0.206338349660117</v>
@@ -3874,7 +3874,7 @@
         <v>0.932094523155001</v>
       </c>
       <c r="C202" t="n">
-        <v>0.1036375577801095</v>
+        <v>0.1033997383818313</v>
       </c>
       <c r="D202" t="n">
         <v>0.2073824008167201</v>
@@ -3891,7 +3891,7 @@
         <v>0.9356171142595333</v>
       </c>
       <c r="C203" t="n">
-        <v>0.1005860181111379</v>
+        <v>0.1003552011484964</v>
       </c>
       <c r="D203" t="n">
         <v>0.1678036855110897</v>
@@ -3908,7 +3908,7 @@
         <v>0.935934306054839</v>
       </c>
       <c r="C204" t="n">
-        <v>0.1055843336019461</v>
+        <v>0.1053420468940897</v>
       </c>
       <c r="D204" t="n">
         <v>0.199907193047198</v>
@@ -3925,7 +3925,7 @@
         <v>0.9362514978501444</v>
       </c>
       <c r="C205" t="n">
-        <v>0.1021199968379685</v>
+        <v>0.1018856598203816</v>
       </c>
       <c r="D205" t="n">
         <v>0.1988781864996311</v>
@@ -3942,7 +3942,7 @@
         <v>0.9425865228730528</v>
       </c>
       <c r="C206" t="n">
-        <v>0.1040434990530923</v>
+        <v>0.1038047481323878</v>
       </c>
       <c r="D206" t="n">
         <v>0.2026339178050436</v>
@@ -3959,7 +3959,7 @@
         <v>0.9489215478959611</v>
       </c>
       <c r="C207" t="n">
-        <v>0.1080595126408094</v>
+        <v>0.1078115460848143</v>
       </c>
       <c r="D207" t="n">
         <v>0.2012811284805402</v>
@@ -3976,7 +3976,7 @@
         <v>0.9523807006414322</v>
       </c>
       <c r="C208" t="n">
-        <v>0.109494028942173</v>
+        <v>0.1092427705698623</v>
       </c>
       <c r="D208" t="n">
         <v>0.1936200511789097</v>
@@ -3993,7 +3993,7 @@
         <v>0.9558398533869034</v>
       </c>
       <c r="C209" t="n">
-        <v>0.1135232012093949</v>
+        <v>0.1132626970062805</v>
       </c>
       <c r="D209" t="n">
         <v>0.1677059179233804</v>
@@ -4010,7 +4010,7 @@
         <v>0.9580460985409177</v>
       </c>
       <c r="C210" t="n">
-        <v>0.1155476758045292</v>
+        <v>0.1152825259947413</v>
       </c>
       <c r="D210" t="n">
         <v>0.1967546241115967</v>
@@ -4027,7 +4027,7 @@
         <v>0.960252343694932</v>
       </c>
       <c r="C211" t="n">
-        <v>0.1147510867570524</v>
+        <v>0.1144877648977875</v>
       </c>
       <c r="D211" t="n">
         <v>0.2062999390740727</v>
@@ -4044,7 +4044,7 @@
         <v>0.9626876718122225</v>
       </c>
       <c r="C212" t="n">
-        <v>0.1123417315570395</v>
+        <v>0.1120839384984929</v>
       </c>
       <c r="D212" t="n">
         <v>0.2034927897551921</v>
@@ -4061,7 +4061,7 @@
         <v>0.9651229999295129</v>
       </c>
       <c r="C213" t="n">
-        <v>0.1105351338718394</v>
+        <v>0.1102814864529976</v>
       </c>
       <c r="D213" t="n">
         <v>0.2056732665313098</v>
@@ -4078,7 +4078,7 @@
         <v>0.9683689293014731</v>
       </c>
       <c r="C214" t="n">
-        <v>0.1111559827488945</v>
+        <v>0.1109009106543894</v>
       </c>
       <c r="D214" t="n">
         <v>0.199407471839572</v>
@@ -4095,7 +4095,7 @@
         <v>0.9716148586734333</v>
       </c>
       <c r="C215" t="n">
-        <v>0.1160953838787606</v>
+        <v>0.115828977231129</v>
       </c>
       <c r="D215" t="n">
         <v>0.1611749744274283</v>
@@ -4112,7 +4112,7 @@
         <v>0.9702685557200252</v>
       </c>
       <c r="C216" t="n">
-        <v>0.1122988056838986</v>
+        <v>0.1120411111283035</v>
       </c>
       <c r="D216" t="n">
         <v>0.2010783497515474</v>
@@ -4129,7 +4129,7 @@
         <v>0.9689222527666174</v>
       </c>
       <c r="C217" t="n">
-        <v>0.1042808127396134</v>
+        <v>0.1040415172499386</v>
       </c>
       <c r="D217" t="n">
         <v>0.2007385003746517</v>
@@ -4146,7 +4146,7 @@
         <v>0.9719761048847536</v>
       </c>
       <c r="C218" t="n">
-        <v>0.09975553875524179</v>
+        <v>0.0995266275119643</v>
       </c>
       <c r="D218" t="n">
         <v>0.1883791166056598</v>
@@ -4163,7 +4163,7 @@
         <v>0.9750299570028899</v>
       </c>
       <c r="C219" t="n">
-        <v>0.0995661715855488</v>
+        <v>0.09933769488730801</v>
       </c>
       <c r="D219" t="n">
         <v>0.2029681227521643</v>
@@ -4180,7 +4180,7 @@
         <v>0.9814090364418128</v>
       </c>
       <c r="C220" t="n">
-        <v>0.102159238683497</v>
+        <v>0.1019248116167785</v>
       </c>
       <c r="D220" t="n">
         <v>0.1962484477402905</v>
@@ -4197,7 +4197,7 @@
         <v>0.9877881158807358</v>
       </c>
       <c r="C221" t="n">
-        <v>0.1182642290607439</v>
+        <v>0.117992845516057</v>
       </c>
       <c r="D221" t="n">
         <v>0.181921605565962</v>
@@ -4214,7 +4214,7 @@
         <v>0.9889881581729753</v>
       </c>
       <c r="C222" t="n">
-        <v>0.1219124809570391</v>
+        <v>0.1216327256879568</v>
       </c>
       <c r="D222" t="n">
         <v>0.1902955039903355</v>
@@ -4231,7 +4231,7 @@
         <v>0.9901882004652146</v>
       </c>
       <c r="C223" t="n">
-        <v>0.1147357643189681</v>
+        <v>0.1144724776204411</v>
       </c>
       <c r="D223" t="n">
         <v>0.2097581044718746</v>
@@ -4248,7 +4248,7 @@
         <v>0.9907009938676252</v>
       </c>
       <c r="C224" t="n">
-        <v>0.1110728672739206</v>
+        <v>0.1108179859063361</v>
       </c>
       <c r="D224" t="n">
         <v>0.2006659943116632</v>
@@ -4265,7 +4265,7 @@
         <v>0.991213787270036</v>
       </c>
       <c r="C225" t="n">
-        <v>0.107595355683794</v>
+        <v>0.1073484542390442</v>
       </c>
       <c r="D225" t="n">
         <v>0.1995533179020576</v>
@@ -4282,7 +4282,7 @@
         <v>0.9958906040741524</v>
       </c>
       <c r="C226" t="n">
-        <v>0.111066415876903</v>
+        <v>0.110811549313482</v>
       </c>
       <c r="D226" t="n">
         <v>0.2073520918414291</v>
@@ -4299,7 +4299,7 @@
         <v>1.000567420878269</v>
       </c>
       <c r="C227" t="n">
-        <v>0.1234099746038231</v>
+        <v>0.1231267830029164</v>
       </c>
       <c r="D227" t="n">
         <v>0.148915502234934</v>
@@ -4316,7 +4316,7 @@
         <v>0.9982642560090224</v>
       </c>
       <c r="C228" t="n">
-        <v>0.1185257303241864</v>
+        <v>0.1182537467067609</v>
       </c>
       <c r="D228" t="n">
         <v>0.2014496650455873</v>
@@ -4333,7 +4333,7 @@
         <v>0.9959610911397758</v>
       </c>
       <c r="C229" t="n">
-        <v>0.108739187668528</v>
+        <v>0.1084896614471994</v>
       </c>
       <c r="D229" t="n">
         <v>0.1922765876133251</v>
@@ -4350,7 +4350,7 @@
         <v>1</v>
       </c>
       <c r="C230" t="n">
-        <v>0.10467</v>
+        <v>0.1044298114337025</v>
       </c>
       <c r="D230" t="n">
         <v>0.1991</v>
@@ -4367,7 +4367,7 @@
         <v>1.004038908860224</v>
       </c>
       <c r="C231" t="n">
-        <v>0.10299401655399</v>
+        <v>0.1027576739040108</v>
       </c>
       <c r="D231" t="n">
         <v>0.215828289210421</v>
@@ -4384,7 +4384,7 @@
         <v>1.000726016775922</v>
       </c>
       <c r="C232" t="n">
-        <v>0.09778900354292716</v>
+        <v>0.09756460495153864</v>
       </c>
       <c r="D232" t="n">
         <v>0.2031525078712149</v>
@@ -4401,7 +4401,7 @@
         <v>0.9974131246916189</v>
       </c>
       <c r="C233" t="n">
-        <v>0.0850299619089348</v>
+        <v>0.08483484177285724</v>
       </c>
       <c r="D233" t="n">
         <v>0.2048298693313923</v>
@@ -4418,7 +4418,7 @@
         <v>1.000636145767251</v>
       </c>
       <c r="C234" t="n">
-        <v>0.08307715082214917</v>
+        <v>0.08288651184490591</v>
       </c>
       <c r="D234" t="n">
         <v>0.1859816885360515</v>
@@ -4435,7 +4435,7 @@
         <v>1.003859166842884</v>
       </c>
       <c r="C235" t="n">
-        <v>0.08881723945442098</v>
+        <v>0.08861342856871296</v>
       </c>
       <c r="D235" t="n">
         <v>0.196342282374006</v>
@@ -4452,7 +4452,7 @@
         <v>1.006595827165715</v>
       </c>
       <c r="C236" t="n">
-        <v>0.09245021436461767</v>
+        <v>0.09223806681095249</v>
       </c>
       <c r="D236" t="n">
         <v>0.1989875127577146</v>
@@ -4469,7 +4469,7 @@
         <v>1.009332487488546</v>
       </c>
       <c r="C237" t="n">
-        <v>0.09380457002388369</v>
+        <v>0.09358931460030301</v>
       </c>
       <c r="D237" t="n">
         <v>0.2049869617442072</v>
@@ -4486,7 +4486,7 @@
         <v>1.010134277860013</v>
       </c>
       <c r="C238" t="n">
-        <v>0.09426469538458317</v>
+        <v>0.09404838410115055</v>
       </c>
       <c r="D238" t="n">
         <v>0.2094771008546293</v>
@@ -4503,7 +4503,7 @@
         <v>1.01093606823148</v>
       </c>
       <c r="C239" t="n">
-        <v>0.09309194019027829</v>
+        <v>0.09287832005415375</v>
       </c>
       <c r="D239" t="n">
         <v>0.2055520685531806</v>
@@ -4520,7 +4520,7 @@
         <v>1.011859448791147</v>
       </c>
       <c r="C240" t="n">
-        <v>0.09235472388150678</v>
+        <v>0.09214279545196727</v>
       </c>
       <c r="D240" t="n">
         <v>0.2193980599432264</v>
@@ -4537,7 +4537,7 @@
         <v>1.012782829350814</v>
       </c>
       <c r="C241" t="n">
-        <v>0.09309991961498709</v>
+        <v>0.09288628116830003</v>
       </c>
       <c r="D241" t="n">
         <v>0.2016226915407824</v>
@@ -4554,7 +4554,7 @@
         <v>1.016774159441743</v>
       </c>
       <c r="C242" t="n">
-        <v>0.09624556160409289</v>
+        <v>0.09602470478309179</v>
       </c>
       <c r="D242" t="n">
         <v>0.2109613014927235</v>
@@ -4571,7 +4571,7 @@
         <v>1.020765489532671</v>
       </c>
       <c r="C243" t="n">
-        <v>0.100924258369241</v>
+        <v>0.1006926652391908</v>
       </c>
       <c r="D243" t="n">
         <v>0.2204228123964203</v>
@@ -4588,7 +4588,7 @@
         <v>1.028945513498273</v>
       </c>
       <c r="C244" t="n">
-        <v>0.1102390734125013</v>
+        <v>0.10998610537015</v>
       </c>
       <c r="D244" t="n">
         <v>0.214199874637356</v>
@@ -4605,7 +4605,7 @@
         <v>1.037125537463875</v>
       </c>
       <c r="C245" t="n">
-        <v>0.1131299883781782</v>
+        <v>0.1128703864892529</v>
       </c>
       <c r="D245" t="n">
         <v>0.2253343414640777</v>
@@ -4622,7 +4622,7 @@
         <v>1.042716923944456</v>
       </c>
       <c r="C246" t="n">
-        <v>0.1170403943750517</v>
+        <v>0.1167718191909127</v>
       </c>
       <c r="D246" t="n">
         <v>0.2180841173458437</v>
@@ -4639,7 +4639,7 @@
         <v>1.048308310425037</v>
       </c>
       <c r="C247" t="n">
-        <v>0.1196785323099577</v>
+        <v>0.1194039033322935</v>
       </c>
       <c r="D247" t="n">
         <v>0.2206411965829207</v>
@@ -4656,7 +4656,7 @@
         <v>1.052481144709946</v>
       </c>
       <c r="C248" t="n">
-        <v>0.1212278249746343</v>
+        <v>0.1209496408007925</v>
       </c>
       <c r="D248" t="n">
         <v>0.213685538339958</v>
@@ -4673,7 +4673,7 @@
         <v>1.056653978994854</v>
       </c>
       <c r="C249" t="n">
-        <v>0.1226229234694728</v>
+        <v>0.1223415379322287</v>
       </c>
       <c r="D249" t="n">
         <v>0.2213591247936227</v>
@@ -4690,7 +4690,7 @@
         <v>1.061901741030521</v>
       </c>
       <c r="C250" t="n">
-        <v>0.121762678225314</v>
+        <v>0.1214832667118767</v>
       </c>
       <c r="D250" t="n">
         <v>0.2212069073095611</v>
@@ -4707,7 +4707,7 @@
         <v>1.067149503066187</v>
       </c>
       <c r="C251" t="n">
-        <v>0.1236940087782743</v>
+        <v>0.1234101653978592</v>
       </c>
       <c r="D251" t="n">
         <v>0.2063440964619394</v>
@@ -4724,7 +4724,7 @@
         <v>1.072992880806372</v>
       </c>
       <c r="C252" t="n">
-        <v>0.1285563049554772</v>
+        <v>0.1282613039563776</v>
       </c>
       <c r="D252" t="n">
         <v>0.2224618674269423</v>
@@ -4741,7 +4741,7 @@
         <v>1.078836258546557</v>
       </c>
       <c r="C253" t="n">
-        <v>0.1278321885341496</v>
+        <v>0.1275388491810333</v>
       </c>
       <c r="D253" t="n">
         <v>0.2167150002123427</v>
@@ -4758,7 +4758,7 @@
         <v>1.087540373782951</v>
       </c>
       <c r="C254" t="n">
-        <v>0.1264504778996333</v>
+        <v>0.1261603091884997</v>
       </c>
       <c r="D254" t="n">
         <v>0.2121300556387827</v>
@@ -4775,7 +4775,7 @@
         <v>1.096244489019346</v>
       </c>
       <c r="C255" t="n">
-        <v>0.1275262967342798</v>
+        <v>0.1272336593178487</v>
       </c>
       <c r="D255" t="n">
         <v>0.2311528153967561</v>
@@ -4792,7 +4792,7 @@
         <v>1.106462653781992</v>
       </c>
       <c r="C256" t="n">
-        <v>0.1533264583491549</v>
+        <v>0.1529746167306744</v>
       </c>
       <c r="D256" t="n">
         <v>0.2383270678848933</v>
@@ -4809,7 +4809,7 @@
         <v>1.116680818544638</v>
       </c>
       <c r="C257" t="n">
-        <v>0.1529174650125631</v>
+        <v>0.1525665619201468</v>
       </c>
       <c r="D257" t="n">
         <v>0.2084749698695519</v>
@@ -4826,7 +4826,7 @@
         <v>1.125836878606931</v>
       </c>
       <c r="C258" t="n">
-        <v>0.156443622825659</v>
+        <v>0.1560846281808431</v>
       </c>
       <c r="D258" t="n">
         <v>0.2416868777088617</v>
@@ -4843,7 +4843,7 @@
         <v>1.134992938669225</v>
       </c>
       <c r="C259" t="n">
-        <v>0.1663622684925166</v>
+        <v>0.1659805133118992</v>
       </c>
       <c r="D259" t="n">
         <v>0.248107270455951</v>
@@ -4860,7 +4860,7 @@
         <v>1.135402138707049</v>
       </c>
       <c r="C260" t="n">
-        <v>0.1558126358661418</v>
+        <v>0.1554550891610714</v>
       </c>
       <c r="D260" t="n">
         <v>0.230579097110146</v>
@@ -4877,7 +4877,7 @@
         <v>1.135811338744872</v>
       </c>
       <c r="C261" t="n">
-        <v>0.1408596608806502</v>
+        <v>0.1405364270983241</v>
       </c>
       <c r="D261" t="n">
         <v>0.2332253526300659</v>
@@ -4894,7 +4894,7 @@
         <v>1.140294553096823</v>
       </c>
       <c r="C262" t="n">
-        <v>0.141410830703414</v>
+        <v>0.1410863321394932</v>
       </c>
       <c r="D262" t="n">
         <v>0.2276604753525971</v>
@@ -4911,7 +4911,7 @@
         <v>1.144777767448774</v>
       </c>
       <c r="C263" t="n">
-        <v>0.1547461918262026</v>
+        <v>0.1543910923138807</v>
       </c>
       <c r="D263" t="n">
         <v>0.2250218403298324</v>
@@ -4928,7 +4928,7 @@
         <v>1.141831939302186</v>
       </c>
       <c r="C264" t="n">
-        <v>0.1359131713331141</v>
+        <v>0.1356012883698635</v>
       </c>
       <c r="D264" t="n">
         <v>0.2235004918113972</v>
@@ -4945,7 +4945,7 @@
         <v>1.138886111155598</v>
       </c>
       <c r="C265" t="n">
-        <v>0.1163768692073303</v>
+        <v>0.1161098166290834</v>
       </c>
       <c r="D265" t="n">
         <v>0.2286444600995081</v>

</xml_diff>

<commit_message>
im not adjusting emissions but am changing scale of the dollars adn uptake is much higher
</commit_message>
<xml_diff>
--- a/package/calibration_data/aligned_data.xlsx
+++ b/package/calibration_data/aligned_data.xlsx
@@ -474,7 +474,7 @@
         <v>0.6292944244731091</v>
       </c>
       <c r="C2" t="n">
-        <v>0.07846883442729451</v>
+        <v>0.07828877025570641</v>
       </c>
       <c r="D2" t="n">
         <v>0.1730509532023567</v>
@@ -491,7 +491,7 @@
         <v>0.6337245365475435</v>
       </c>
       <c r="C3" t="n">
-        <v>0.07962450100938197</v>
+        <v>0.07944178490410254</v>
       </c>
       <c r="D3" t="n">
         <v>0.1757861556172246</v>
@@ -508,7 +508,7 @@
         <v>0.6358426728695283</v>
       </c>
       <c r="C4" t="n">
-        <v>0.08200141674149457</v>
+        <v>0.08181324627506194</v>
       </c>
       <c r="D4" t="n">
         <v>0.1775596461471948</v>
@@ -525,7 +525,7 @@
         <v>0.6379608091915133</v>
       </c>
       <c r="C5" t="n">
-        <v>0.08638461674446869</v>
+        <v>0.08618638805194923</v>
       </c>
       <c r="D5" t="n">
         <v>0.1746188768886557</v>
@@ -542,7 +542,7 @@
         <v>0.6417406780855712</v>
       </c>
       <c r="C6" t="n">
-        <v>0.09316847449715111</v>
+        <v>0.09295467873605819</v>
       </c>
       <c r="D6" t="n">
         <v>0.1865239404132629</v>
@@ -559,7 +559,7 @@
         <v>0.6455205469796292</v>
       </c>
       <c r="C7" t="n">
-        <v>0.09178638894955229</v>
+        <v>0.09157576469076356</v>
       </c>
       <c r="D7" t="n">
         <v>0.1993739790347238</v>
@@ -576,7 +576,7 @@
         <v>0.6449777965743286</v>
       </c>
       <c r="C8" t="n">
-        <v>0.08451453722828758</v>
+        <v>0.08432059984863574</v>
       </c>
       <c r="D8" t="n">
         <v>0.2023325464738861</v>
@@ -593,7 +593,7 @@
         <v>0.644435046169028</v>
       </c>
       <c r="C9" t="n">
-        <v>0.07485626408242731</v>
+        <v>0.07468448975598854</v>
       </c>
       <c r="D9" t="n">
         <v>0.1986235862883644</v>
@@ -610,7 +610,7 @@
         <v>0.6447099457249594</v>
       </c>
       <c r="C10" t="n">
-        <v>0.07947760126824469</v>
+        <v>0.07929522225705347</v>
       </c>
       <c r="D10" t="n">
         <v>0.1996246542393265</v>
@@ -627,7 +627,7 @@
         <v>0.644984845280891</v>
       </c>
       <c r="C11" t="n">
-        <v>0.07404825144255989</v>
+        <v>0.07387833128061448</v>
       </c>
       <c r="D11" t="n">
         <v>0.1936479607448855</v>
@@ -644,7 +644,7 @@
         <v>0.6429213364347642</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0654667960366731</v>
+        <v>0.06531656793043313</v>
       </c>
       <c r="D12" t="n">
         <v>0.1885145089010402</v>
@@ -661,7 +661,7 @@
         <v>0.6408578275886374</v>
       </c>
       <c r="C13" t="n">
-        <v>0.05636195493766395</v>
+        <v>0.05623261991186667</v>
       </c>
       <c r="D13" t="n">
         <v>0.1913060818205316</v>
@@ -678,7 +678,7 @@
         <v>0.6448562063861281</v>
       </c>
       <c r="C14" t="n">
-        <v>0.05726858117247768</v>
+        <v>0.05713716569138751</v>
       </c>
       <c r="D14" t="n">
         <v>0.202060550413589</v>
@@ -695,7 +695,7 @@
         <v>0.6488545851836187</v>
       </c>
       <c r="C15" t="n">
-        <v>0.06098438834149893</v>
+        <v>0.06084444611543344</v>
       </c>
       <c r="D15" t="n">
         <v>0.1938801125438606</v>
@@ -712,7 +712,7 @@
         <v>0.6523384084020581</v>
       </c>
       <c r="C16" t="n">
-        <v>0.06930451958323991</v>
+        <v>0.06914548496781395</v>
       </c>
       <c r="D16" t="n">
         <v>0.1928446928460867</v>
@@ -729,7 +729,7 @@
         <v>0.6558222316204976</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0757979793962909</v>
+        <v>0.07562404409487271</v>
       </c>
       <c r="D17" t="n">
         <v>0.183738815474815</v>
@@ -746,7 +746,7 @@
         <v>0.6555755268908156</v>
       </c>
       <c r="C18" t="n">
-        <v>0.07399605081365281</v>
+        <v>0.07382625043764623</v>
       </c>
       <c r="D18" t="n">
         <v>0.1955533645497895</v>
@@ -763,7 +763,7 @@
         <v>0.6553288221611334</v>
       </c>
       <c r="C19" t="n">
-        <v>0.07475636404704668</v>
+        <v>0.0745848189634308</v>
       </c>
       <c r="D19" t="n">
         <v>0.1963899582130008</v>
@@ -780,7 +780,7 @@
         <v>0.6568196235990695</v>
       </c>
       <c r="C20" t="n">
-        <v>0.07527180708927593</v>
+        <v>0.07509907920709961</v>
       </c>
       <c r="D20" t="n">
         <v>0.2021864073919063</v>
@@ -797,7 +797,7 @@
         <v>0.6583104250370057</v>
       </c>
       <c r="C21" t="n">
-        <v>0.07460006424361178</v>
+        <v>0.07442887782461517</v>
       </c>
       <c r="D21" t="n">
         <v>0.1962599938968569</v>
@@ -814,7 +814,7 @@
         <v>0.6596021005145555</v>
       </c>
       <c r="C22" t="n">
-        <v>0.07399915791948407</v>
+        <v>0.07382935041353296</v>
       </c>
       <c r="D22" t="n">
         <v>0.1760152066062713</v>
@@ -831,7 +831,7 @@
         <v>0.6608937759921054</v>
       </c>
       <c r="C23" t="n">
-        <v>0.07167566365546442</v>
+        <v>0.07151118792324097</v>
       </c>
       <c r="D23" t="n">
         <v>0.1812696750247971</v>
@@ -848,7 +848,7 @@
         <v>0.660273489814619</v>
       </c>
       <c r="C24" t="n">
-        <v>0.07378760582024704</v>
+        <v>0.07361828376758162</v>
       </c>
       <c r="D24" t="n">
         <v>0.1900727530878695</v>
@@ -865,7 +865,7 @@
         <v>0.6596532036371325</v>
       </c>
       <c r="C25" t="n">
-        <v>0.07208333066196505</v>
+        <v>0.07191791944723643</v>
       </c>
       <c r="D25" t="n">
         <v>0.2017726879307581</v>
@@ -882,7 +882,7 @@
         <v>0.6655582575597377</v>
       </c>
       <c r="C26" t="n">
-        <v>0.07491455396077745</v>
+        <v>0.07474264587526436</v>
       </c>
       <c r="D26" t="n">
         <v>0.1924700032566304</v>
@@ -899,7 +899,7 @@
         <v>0.671463311482343</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0827893334593037</v>
+        <v>0.08259935494293497</v>
       </c>
       <c r="D27" t="n">
         <v>0.1848202245421765</v>
@@ -916,7 +916,7 @@
         <v>0.6725593853527877</v>
       </c>
       <c r="C28" t="n">
-        <v>0.09590231198121908</v>
+        <v>0.09568224282272683</v>
       </c>
       <c r="D28" t="n">
         <v>0.1697991322210112</v>
@@ -933,7 +933,7 @@
         <v>0.6736554592232326</v>
       </c>
       <c r="C29" t="n">
-        <v>0.09316335099899029</v>
+        <v>0.09294956699490202</v>
       </c>
       <c r="D29" t="n">
         <v>0.1857032378899567</v>
@@ -950,7 +950,7 @@
         <v>0.6715285120180446</v>
       </c>
       <c r="C30" t="n">
-        <v>0.08443424066925756</v>
+        <v>0.08424048754789741</v>
       </c>
       <c r="D30" t="n">
         <v>0.1897164419975911</v>
@@ -967,7 +967,7 @@
         <v>0.6694015648128568</v>
       </c>
       <c r="C31" t="n">
-        <v>0.08107241281273692</v>
+        <v>0.0808863741521869</v>
       </c>
       <c r="D31" t="n">
         <v>0.1959959565327268</v>
@@ -984,7 +984,7 @@
         <v>0.6701222950588567</v>
       </c>
       <c r="C32" t="n">
-        <v>0.08008985881492896</v>
+        <v>0.07990607484279055</v>
       </c>
       <c r="D32" t="n">
         <v>0.201455765604908</v>
@@ -1001,7 +1001,7 @@
         <v>0.6708430253048565</v>
       </c>
       <c r="C33" t="n">
-        <v>0.08554907457511361</v>
+        <v>0.08535276321970831</v>
       </c>
       <c r="D33" t="n">
         <v>0.1922953584281174</v>
@@ -1018,7 +1018,7 @@
         <v>0.671923239585536</v>
       </c>
       <c r="C34" t="n">
-        <v>0.09233197535817972</v>
+        <v>0.09212009913018031</v>
       </c>
       <c r="D34" t="n">
         <v>0.1500171359784738</v>
@@ -1035,7 +1035,7 @@
         <v>0.6730034538662155</v>
       </c>
       <c r="C35" t="n">
-        <v>0.08197580515087087</v>
+        <v>0.08178769345592227</v>
       </c>
       <c r="D35" t="n">
         <v>0.1555712669801737</v>
@@ -1052,7 +1052,7 @@
         <v>0.6714774088954677</v>
       </c>
       <c r="C36" t="n">
-        <v>0.07773902637449152</v>
+        <v>0.07756063690959947</v>
       </c>
       <c r="D36" t="n">
         <v>0.1867523737042383</v>
@@ -1069,7 +1069,7 @@
         <v>0.6699513639247199</v>
       </c>
       <c r="C37" t="n">
-        <v>0.07527412095196009</v>
+        <v>0.07510138776011185</v>
       </c>
       <c r="D37" t="n">
         <v>0.1858343854554637</v>
@@ -1086,7 +1086,7 @@
         <v>0.6752572777895257</v>
       </c>
       <c r="C38" t="n">
-        <v>0.07650417359307922</v>
+        <v>0.07632861777220316</v>
       </c>
       <c r="D38" t="n">
         <v>0.1864474536463158</v>
@@ -1103,7 +1103,7 @@
         <v>0.6805631916543314</v>
       </c>
       <c r="C39" t="n">
-        <v>0.08437129821908514</v>
+        <v>0.08417768953315889</v>
       </c>
       <c r="D39" t="n">
         <v>0.182055100127911</v>
@@ -1120,7 +1120,7 @@
         <v>0.6828381616973286</v>
       </c>
       <c r="C40" t="n">
-        <v>0.09415115265408505</v>
+        <v>0.09393510191966982</v>
       </c>
       <c r="D40" t="n">
         <v>0.1777873686764026</v>
@@ -1137,7 +1137,7 @@
         <v>0.6851131317403256</v>
       </c>
       <c r="C41" t="n">
-        <v>0.09567762893916479</v>
+        <v>0.09545807536582342</v>
       </c>
       <c r="D41" t="n">
         <v>0.1668337603012439</v>
@@ -1154,7 +1154,7 @@
         <v>0.6876700500458166</v>
       </c>
       <c r="C42" t="n">
-        <v>0.1002515668603087</v>
+        <v>0.1000215173703569</v>
       </c>
       <c r="D42" t="n">
         <v>0.174066036454583</v>
@@ -1171,7 +1171,7 @@
         <v>0.6902269683513075</v>
       </c>
       <c r="C43" t="n">
-        <v>0.1009233240572902</v>
+        <v>0.1006917330712264</v>
       </c>
       <c r="D43" t="n">
         <v>0.1796510505757104</v>
@@ -1188,7 +1188,7 @@
         <v>0.6893370691478113</v>
       </c>
       <c r="C44" t="n">
-        <v>0.09718032439894168</v>
+        <v>0.09695732255706047</v>
       </c>
       <c r="D44" t="n">
         <v>0.1768365658192415</v>
@@ -1205,7 +1205,7 @@
         <v>0.6884471699443152</v>
       </c>
       <c r="C45" t="n">
-        <v>0.09286115593324459</v>
+        <v>0.09264806538286402</v>
       </c>
       <c r="D45" t="n">
         <v>0.1815680352206409</v>
@@ -1222,7 +1222,7 @@
         <v>0.6931944738140552</v>
       </c>
       <c r="C46" t="n">
-        <v>0.09153275508803327</v>
+        <v>0.09132271284848179</v>
       </c>
       <c r="D46" t="n">
         <v>0.1757082674503145</v>
@@ -1239,7 +1239,7 @@
         <v>0.697941777683795</v>
       </c>
       <c r="C47" t="n">
-        <v>0.1021288627205429</v>
+        <v>0.101894505358219</v>
       </c>
       <c r="D47" t="n">
         <v>0.1637672419887494</v>
@@ -1256,7 +1256,7 @@
         <v>0.696169027983365</v>
       </c>
       <c r="C48" t="n">
-        <v>0.1012685097528996</v>
+        <v>0.1010361266615779</v>
       </c>
       <c r="D48" t="n">
         <v>0.1795540953065595</v>
@@ -1273,7 +1273,7 @@
         <v>0.694396278282935</v>
       </c>
       <c r="C49" t="n">
-        <v>0.09258402156038735</v>
+        <v>0.09237156695638767</v>
       </c>
       <c r="D49" t="n">
         <v>0.1785723856507705</v>
@@ -1290,7 +1290,7 @@
         <v>0.6979999295129343</v>
       </c>
       <c r="C50" t="n">
-        <v>0.08664757321996157</v>
+        <v>0.08644874111539617</v>
       </c>
       <c r="D50" t="n">
         <v>0.1746418514469794</v>
@@ -1307,7 +1307,7 @@
         <v>0.7016035807429337</v>
       </c>
       <c r="C51" t="n">
-        <v>0.0924881254615141</v>
+        <v>0.09227589091241556</v>
       </c>
       <c r="D51" t="n">
         <v>0.1757402661335289</v>
@@ -1324,7 +1324,7 @@
         <v>0.7067826178896173</v>
       </c>
       <c r="C52" t="n">
-        <v>0.09957800067317402</v>
+        <v>0.09934949683046396</v>
       </c>
       <c r="D52" t="n">
         <v>0.1595964546168518</v>
@@ -1341,7 +1341,7 @@
         <v>0.7119616550363008</v>
       </c>
       <c r="C53" t="n">
-        <v>0.1093879135892917</v>
+        <v>0.1091368987222306</v>
       </c>
       <c r="D53" t="n">
         <v>0.1702338870958161</v>
@@ -1358,7 +1358,7 @@
         <v>0.7107457531542962</v>
       </c>
       <c r="C54" t="n">
-        <v>0.1063671498063639</v>
+        <v>0.1061230667528325</v>
       </c>
       <c r="D54" t="n">
         <v>0.1768564911462956</v>
@@ -1375,7 +1375,7 @@
         <v>0.7095298512722915</v>
       </c>
       <c r="C55" t="n">
-        <v>0.1018984611716554</v>
+        <v>0.1016646325168666</v>
       </c>
       <c r="D55" t="n">
         <v>0.1888574522406891</v>
@@ -1392,7 +1392,7 @@
         <v>0.7134295481779093</v>
       </c>
       <c r="C56" t="n">
-        <v>0.1076069812304098</v>
+        <v>0.1073600531082608</v>
       </c>
       <c r="D56" t="n">
         <v>0.1844611010801345</v>
@@ -1409,7 +1409,7 @@
         <v>0.7173292450835271</v>
       </c>
       <c r="C57" t="n">
-        <v>0.1137971169577714</v>
+        <v>0.1135359841941249</v>
       </c>
       <c r="D57" t="n">
         <v>0.1872222566143415</v>
@@ -1426,7 +1426,7 @@
         <v>0.7235321068583915</v>
       </c>
       <c r="C58" t="n">
-        <v>0.1257166048856523</v>
+        <v>0.1254281202091713</v>
       </c>
       <c r="D58" t="n">
         <v>0.1677879928882827</v>
@@ -1443,7 +1443,7 @@
         <v>0.7297349686332558</v>
       </c>
       <c r="C59" t="n">
-        <v>0.1202902475187752</v>
+        <v>0.1200142148246785</v>
       </c>
       <c r="D59" t="n">
         <v>0.1548507401415083</v>
@@ -1460,7 +1460,7 @@
         <v>0.7247198139141467</v>
       </c>
       <c r="C60" t="n">
-        <v>0.1063859418767507</v>
+        <v>0.1061418157006392</v>
       </c>
       <c r="D60" t="n">
         <v>0.1766199813258637</v>
@@ -1477,7 +1477,7 @@
         <v>0.7197046591950377</v>
       </c>
       <c r="C61" t="n">
-        <v>0.09666465141105436</v>
+        <v>0.09644283289539496</v>
       </c>
       <c r="D61" t="n">
         <v>0.1793791360811717</v>
@@ -1494,7 +1494,7 @@
         <v>0.7261189821667724</v>
       </c>
       <c r="C62" t="n">
-        <v>0.1001488761290886</v>
+        <v>0.09991906228583122</v>
       </c>
       <c r="D62" t="n">
         <v>0.1809620781540462</v>
@@ -1511,7 +1511,7 @@
         <v>0.732533305138507</v>
       </c>
       <c r="C63" t="n">
-        <v>0.1040225740802217</v>
+        <v>0.1037838711765157</v>
       </c>
       <c r="D63" t="n">
         <v>0.1836093991311</v>
@@ -1528,7 +1528,7 @@
         <v>0.7371537322901247</v>
       </c>
       <c r="C64" t="n">
-        <v>0.1067891222030981</v>
+        <v>0.1065440708401657</v>
       </c>
       <c r="D64" t="n">
         <v>0.1861212851405623</v>
@@ -1545,7 +1545,7 @@
         <v>0.7417741594417424</v>
       </c>
       <c r="C65" t="n">
-        <v>0.1182974614079849</v>
+        <v>0.1180260016042951</v>
       </c>
       <c r="D65" t="n">
         <v>0.1886018786436136</v>
@@ -1562,7 +1562,7 @@
         <v>0.7426076689927398</v>
       </c>
       <c r="C66" t="n">
-        <v>0.1348087343829717</v>
+        <v>0.1344993857956417</v>
       </c>
       <c r="D66" t="n">
         <v>0.189063493231138</v>
@@ -1579,7 +1579,7 @@
         <v>0.7434411785437371</v>
       </c>
       <c r="C67" t="n">
-        <v>0.1315504209648058</v>
+        <v>0.1312485493014126</v>
       </c>
       <c r="D67" t="n">
         <v>0.2040511130916262</v>
@@ -1596,7 +1596,7 @@
         <v>0.7453055614294777</v>
       </c>
       <c r="C68" t="n">
-        <v>0.1312213474060518</v>
+        <v>0.1309202308750393</v>
       </c>
       <c r="D68" t="n">
         <v>0.2233983061667447</v>
@@ -1613,7 +1613,7 @@
         <v>0.7471699443152182</v>
       </c>
       <c r="C69" t="n">
-        <v>0.1289666437109084</v>
+        <v>0.1286707010983821</v>
       </c>
       <c r="D69" t="n">
         <v>0.1992853180630371</v>
@@ -1630,7 +1630,7 @@
         <v>0.746739973214915</v>
       </c>
       <c r="C70" t="n">
-        <v>0.117992879932037</v>
+        <v>0.1177221190582032</v>
       </c>
       <c r="D70" t="n">
         <v>0.1951147725127431</v>
@@ -1647,7 +1647,7 @@
         <v>0.746310002114612</v>
       </c>
       <c r="C71" t="n">
-        <v>0.1042328252061315</v>
+        <v>0.1039936398345122</v>
       </c>
       <c r="D71" t="n">
         <v>0.1634709432465361</v>
@@ -1664,7 +1664,7 @@
         <v>0.7450095157538592</v>
       </c>
       <c r="C72" t="n">
-        <v>0.1009919986375828</v>
+        <v>0.1007602500624392</v>
       </c>
       <c r="D72" t="n">
         <v>0.1942257071086953</v>
@@ -1681,7 +1681,7 @@
         <v>0.7437090293931063</v>
       </c>
       <c r="C73" t="n">
-        <v>0.1043553284048905</v>
+        <v>0.1041158619224689</v>
       </c>
       <c r="D73" t="n">
         <v>0.1945653397782201</v>
@@ -1698,7 +1698,7 @@
         <v>0.7505638965249877</v>
       </c>
       <c r="C74" t="n">
-        <v>0.1045613842650201</v>
+        <v>0.1043214449416543</v>
       </c>
       <c r="D74" t="n">
         <v>0.199583274246942</v>
@@ -1715,7 +1715,7 @@
         <v>0.7574187636568689</v>
       </c>
       <c r="C75" t="n">
-        <v>0.1074570685403192</v>
+        <v>0.1072104844261391</v>
       </c>
       <c r="D75" t="n">
         <v>0.1872147968917222</v>
@@ -1732,7 +1732,7 @@
         <v>0.7623422851906676</v>
       </c>
       <c r="C76" t="n">
-        <v>0.1221892079313198</v>
+        <v>0.1219088176507232</v>
       </c>
       <c r="D76" t="n">
         <v>0.1812833981332088</v>
@@ -1749,7 +1749,7 @@
         <v>0.7672658067244661</v>
       </c>
       <c r="C77" t="n">
-        <v>0.1305544950942564</v>
+        <v>0.1302549088040072</v>
       </c>
       <c r="D77" t="n">
         <v>0.1790774446036821</v>
@@ -1766,7 +1766,7 @@
         <v>0.7667371537322901</v>
       </c>
       <c r="C78" t="n">
-        <v>0.1363570285997959</v>
+        <v>0.1360441271074488</v>
       </c>
       <c r="D78" t="n">
         <v>0.1845482500896329</v>
@@ -1783,7 +1783,7 @@
         <v>0.7662085007401142</v>
       </c>
       <c r="C79" t="n">
-        <v>0.1303431114422918</v>
+        <v>0.1300440102187886</v>
       </c>
       <c r="D79" t="n">
         <v>0.1921148092951372</v>
@@ -1800,7 +1800,7 @@
         <v>0.7663424261647988</v>
       </c>
       <c r="C80" t="n">
-        <v>0.1242525491855299</v>
+        <v>0.1239674241100768</v>
       </c>
       <c r="D80" t="n">
         <v>0.197431324215193</v>
@@ -1817,7 +1817,7 @@
         <v>0.7664763515894832</v>
       </c>
       <c r="C81" t="n">
-        <v>0.115385164612838</v>
+        <v>0.1151203877210795</v>
       </c>
       <c r="D81" t="n">
         <v>0.1971358929556741</v>
@@ -1834,7 +1834,7 @@
         <v>0.7690826108409106</v>
       </c>
       <c r="C82" t="n">
-        <v>0.1139799532122473</v>
+        <v>0.1137184008901999</v>
       </c>
       <c r="D82" t="n">
         <v>0.1963378158230589</v>
@@ -1851,7 +1851,7 @@
         <v>0.771688870092338</v>
       </c>
       <c r="C83" t="n">
-        <v>0.1209814001708082</v>
+        <v>0.1207037814734194</v>
       </c>
       <c r="D83" t="n">
         <v>0.1623711379756027</v>
@@ -1868,7 +1868,7 @@
         <v>0.7728060900824699</v>
       </c>
       <c r="C84" t="n">
-        <v>0.1317536200952225</v>
+        <v>0.131451282146286</v>
       </c>
       <c r="D84" t="n">
         <v>0.1859457396158266</v>
@@ -1885,7 +1885,7 @@
         <v>0.7739233100726016</v>
       </c>
       <c r="C85" t="n">
-        <v>0.1299741184828296</v>
+        <v>0.1296758639956397</v>
       </c>
       <c r="D85" t="n">
         <v>0.1868402180397372</v>
@@ -1902,7 +1902,7 @@
         <v>0.7770317896665961</v>
       </c>
       <c r="C86" t="n">
-        <v>0.1272534808935253</v>
+        <v>0.126961469513644</v>
       </c>
       <c r="D86" t="n">
         <v>0.1766980473976641</v>
@@ -1919,7 +1919,7 @@
         <v>0.7801402692605907</v>
       </c>
       <c r="C87" t="n">
-        <v>0.1242468871551385</v>
+        <v>0.1239617750724718</v>
       </c>
       <c r="D87" t="n">
         <v>0.1712512547604096</v>
@@ -1936,7 +1936,7 @@
         <v>0.7853668851765701</v>
       </c>
       <c r="C88" t="n">
-        <v>0.1378591357027464</v>
+        <v>0.1375427872919748</v>
       </c>
       <c r="D88" t="n">
         <v>0.1674376682821756</v>
@@ -1953,7 +1953,7 @@
         <v>0.7905935010925496</v>
       </c>
       <c r="C89" t="n">
-        <v>0.1459409922299541</v>
+        <v>0.1456060982040847</v>
       </c>
       <c r="D89" t="n">
         <v>0.1635480178135991</v>
@@ -1970,7 +1970,7 @@
         <v>0.797643969831536</v>
       </c>
       <c r="C90" t="n">
-        <v>0.1510072219632517</v>
+        <v>0.1506607023478516</v>
       </c>
       <c r="D90" t="n">
         <v>0.1698752891325912</v>
@@ -1987,7 +1987,7 @@
         <v>0.8046944385705224</v>
       </c>
       <c r="C91" t="n">
-        <v>0.168921261890997</v>
+        <v>0.1685336345315744</v>
       </c>
       <c r="D91" t="n">
         <v>0.1801926210122457</v>
@@ -2004,7 +2004,7 @@
         <v>0.8041657855783464</v>
       </c>
       <c r="C92" t="n">
-        <v>0.1682861947461148</v>
+        <v>0.1679000246893294</v>
       </c>
       <c r="D92" t="n">
         <v>0.1790675537090115</v>
@@ -2021,7 +2021,7 @@
         <v>0.8036371325861704</v>
       </c>
       <c r="C93" t="n">
-        <v>0.1540994000631512</v>
+        <v>0.1537457847582074</v>
       </c>
       <c r="D93" t="n">
         <v>0.1811762972318703</v>
@@ -2038,7 +2038,7 @@
         <v>0.8010784521040389</v>
       </c>
       <c r="C94" t="n">
-        <v>0.1438810389884645</v>
+        <v>0.1435508719829038</v>
       </c>
       <c r="D94" t="n">
         <v>0.1750140696354565</v>
@@ -2055,7 +2055,7 @@
         <v>0.7985197716219073</v>
       </c>
       <c r="C95" t="n">
-        <v>0.1292391292834066</v>
+        <v>0.1289425613922046</v>
       </c>
       <c r="D95" t="n">
         <v>0.1639283141782744</v>
@@ -2072,7 +2072,7 @@
         <v>0.7865422569958412</v>
       </c>
       <c r="C96" t="n">
-        <v>0.09562105447107296</v>
+        <v>0.09540163072041601</v>
       </c>
       <c r="D96" t="n">
         <v>0.1807913036269987</v>
@@ -2089,7 +2089,7 @@
         <v>0.7745647423697751</v>
       </c>
       <c r="C97" t="n">
-        <v>0.07246650528950062</v>
+        <v>0.07230021479547105</v>
       </c>
       <c r="D97" t="n">
         <v>0.1768735297463315</v>
@@ -2106,7 +2106,7 @@
         <v>0.7788045393670262</v>
       </c>
       <c r="C98" t="n">
-        <v>0.07900570283014599</v>
+        <v>0.07882440669474808</v>
       </c>
       <c r="D98" t="n">
         <v>0.1887508258740689</v>
@@ -2123,7 +2123,7 @@
         <v>0.7830443363642772</v>
       </c>
       <c r="C99" t="n">
-        <v>0.08677669557702954</v>
+        <v>0.08657756717253273</v>
       </c>
       <c r="D99" t="n">
         <v>0.1805772590815596</v>
@@ -2140,7 +2140,7 @@
         <v>0.7843042926622964</v>
       </c>
       <c r="C100" t="n">
-        <v>0.08564278001334601</v>
+        <v>0.08544625362999703</v>
       </c>
       <c r="D100" t="n">
         <v>0.1802871682877345</v>
@@ -2157,7 +2157,7 @@
         <v>0.7855642489603157</v>
       </c>
       <c r="C101" t="n">
-        <v>0.090775515935683</v>
+        <v>0.09056721134957899</v>
       </c>
       <c r="D101" t="n">
         <v>0.1777066614026273</v>
@@ -2174,7 +2174,7 @@
         <v>0.7892612955522661</v>
       </c>
       <c r="C102" t="n">
-        <v>0.09620388131014312</v>
+        <v>0.09598312013383532</v>
       </c>
       <c r="D102" t="n">
         <v>0.190177829377749</v>
@@ -2191,7 +2191,7 @@
         <v>0.7929583421442165</v>
       </c>
       <c r="C103" t="n">
-        <v>0.1123262033654231</v>
+        <v>0.1120684459397616</v>
       </c>
       <c r="D103" t="n">
         <v>0.1862645137203659</v>
@@ -2208,7 +2208,7 @@
         <v>0.7937407485726369</v>
       </c>
       <c r="C104" t="n">
-        <v>0.1103634910485933</v>
+        <v>0.110110237502338</v>
       </c>
       <c r="D104" t="n">
         <v>0.1972936381074169</v>
@@ -2225,7 +2225,7 @@
         <v>0.7945231550010572</v>
       </c>
       <c r="C105" t="n">
-        <v>0.1154277246959253</v>
+        <v>0.1151628501406019</v>
       </c>
       <c r="D105" t="n">
         <v>0.2004976179703511</v>
@@ -2242,7 +2242,7 @@
         <v>0.7955751744554873</v>
       </c>
       <c r="C106" t="n">
-        <v>0.1194984497411805</v>
+        <v>0.1192242340029737</v>
       </c>
       <c r="D106" t="n">
         <v>0.1952046833365451</v>
@@ -2259,7 +2259,7 @@
         <v>0.7966271939099175</v>
       </c>
       <c r="C107" t="n">
-        <v>0.1153111526975911</v>
+        <v>0.1150465456426131</v>
       </c>
       <c r="D107" t="n">
         <v>0.1738579865949963</v>
@@ -2276,7 +2276,7 @@
         <v>0.7936561640938887</v>
       </c>
       <c r="C108" t="n">
-        <v>0.1136260311201108</v>
+        <v>0.1133652909509237</v>
       </c>
       <c r="D108" t="n">
         <v>0.1708548438665672</v>
@@ -2293,7 +2293,7 @@
         <v>0.7906851342778599</v>
       </c>
       <c r="C109" t="n">
-        <v>0.1124594306192584</v>
+        <v>0.112201367474068</v>
       </c>
       <c r="D109" t="n">
         <v>0.1862941310190819</v>
@@ -2310,7 +2310,7 @@
         <v>0.7929354338478889</v>
       </c>
       <c r="C110" t="n">
-        <v>0.1159615223067948</v>
+        <v>0.115695422834276</v>
       </c>
       <c r="D110" t="n">
         <v>0.1914405555864215</v>
@@ -2327,7 +2327,7 @@
         <v>0.7951857334179178</v>
       </c>
       <c r="C111" t="n">
-        <v>0.1129170157694592</v>
+        <v>0.1126579025934942</v>
       </c>
       <c r="D111" t="n">
         <v>0.1787003891395495</v>
@@ -2344,7 +2344,7 @@
         <v>0.7976192993585678</v>
       </c>
       <c r="C112" t="n">
-        <v>0.116747425839477</v>
+        <v>0.1164795229367226</v>
       </c>
       <c r="D112" t="n">
         <v>0.1853014340536372</v>
@@ -2361,7 +2361,7 @@
         <v>0.8000528652992176</v>
       </c>
       <c r="C113" t="n">
-        <v>0.1176672243587202</v>
+        <v>0.1173972107739402</v>
       </c>
       <c r="D113" t="n">
         <v>0.1738635108168471</v>
@@ -2378,7 +2378,7 @@
         <v>0.8002396560231197</v>
       </c>
       <c r="C114" t="n">
-        <v>0.1175647811151238</v>
+        <v>0.1172950026091228</v>
       </c>
       <c r="D114" t="n">
         <v>0.1861942217915969</v>
@@ -2395,7 +2395,7 @@
         <v>0.8004264467470219</v>
       </c>
       <c r="C115" t="n">
-        <v>0.1174623856846592</v>
+        <v>0.1171928421477194</v>
       </c>
       <c r="D115" t="n">
         <v>0.187400104793649</v>
@@ -2412,7 +2412,7 @@
         <v>0.8009339536195108</v>
       </c>
       <c r="C116" t="n">
-        <v>0.1187738384296193</v>
+        <v>0.1185012854730314</v>
       </c>
       <c r="D116" t="n">
         <v>0.1876559225898432</v>
@@ -2429,7 +2429,7 @@
         <v>0.8014414604919997</v>
       </c>
       <c r="C117" t="n">
-        <v>0.119260114071618</v>
+        <v>0.1189864452475486</v>
       </c>
       <c r="D117" t="n">
         <v>0.1895334936961579</v>
@@ -2446,7 +2446,7 @@
         <v>0.8020335518432368</v>
       </c>
       <c r="C118" t="n">
-        <v>0.1146086716556297</v>
+        <v>0.114345676599451</v>
       </c>
       <c r="D118" t="n">
         <v>0.1851543487909162</v>
@@ -2463,7 +2463,7 @@
         <v>0.8026256431944737</v>
       </c>
       <c r="C119" t="n">
-        <v>0.1175890663352903</v>
+        <v>0.1173192321014569</v>
       </c>
       <c r="D119" t="n">
         <v>0.1757980214018803</v>
@@ -2480,7 +2480,7 @@
         <v>0.8021850990343271</v>
       </c>
       <c r="C120" t="n">
-        <v>0.1198601172170184</v>
+        <v>0.1195850715524478</v>
       </c>
       <c r="D120" t="n">
         <v>0.1828754986556069</v>
@@ -2497,7 +2497,7 @@
         <v>0.8017445548741805</v>
       </c>
       <c r="C121" t="n">
-        <v>0.1233684711653853</v>
+        <v>0.1230853748033376</v>
       </c>
       <c r="D121" t="n">
         <v>0.1865930976275568</v>
@@ -2514,7 +2514,7 @@
         <v>0.8067685204764925</v>
       </c>
       <c r="C122" t="n">
-        <v>0.1260212779992355</v>
+        <v>0.1257320941826155</v>
       </c>
       <c r="D122" t="n">
         <v>0.1889017681428494</v>
@@ -2531,7 +2531,7 @@
         <v>0.8117924860788045</v>
       </c>
       <c r="C123" t="n">
-        <v>0.1321519992359055</v>
+        <v>0.1318487471175352</v>
       </c>
       <c r="D123" t="n">
         <v>0.1771388654933185</v>
@@ -2548,7 +2548,7 @@
         <v>0.8184447028970184</v>
       </c>
       <c r="C124" t="n">
-        <v>0.1466928670624027</v>
+        <v>0.1463562476927095</v>
       </c>
       <c r="D124" t="n">
         <v>0.1743550902032722</v>
@@ -2565,7 +2565,7 @@
         <v>0.8250969197152322</v>
       </c>
       <c r="C125" t="n">
-        <v>0.1529274888622161</v>
+        <v>0.1525765627678501</v>
       </c>
       <c r="D125" t="n">
         <v>0.1711314108998646</v>
@@ -2582,7 +2582,7 @@
         <v>0.8236378374568267</v>
       </c>
       <c r="C126" t="n">
-        <v>0.1540361482077373</v>
+        <v>0.1536826780482264</v>
       </c>
       <c r="D126" t="n">
         <v>0.177505201134793</v>
@@ -2599,7 +2599,7 @@
         <v>0.8221787551984211</v>
       </c>
       <c r="C127" t="n">
-        <v>0.1446765672889384</v>
+        <v>0.1443445747669744</v>
       </c>
       <c r="D127" t="n">
         <v>0.1801311443084639</v>
@@ -2616,7 +2616,7 @@
         <v>0.822127652075844</v>
       </c>
       <c r="C128" t="n">
-        <v>0.1402701876148077</v>
+        <v>0.1399483065098351</v>
       </c>
       <c r="D128" t="n">
         <v>0.1909679106445093</v>
@@ -2633,7 +2633,7 @@
         <v>0.8220765489532671</v>
       </c>
       <c r="C129" t="n">
-        <v>0.1395125553040436</v>
+        <v>0.1391924127547078</v>
       </c>
       <c r="D129" t="n">
         <v>0.1842894073464348</v>
@@ -2650,7 +2650,7 @@
         <v>0.8239462183689292</v>
       </c>
       <c r="C130" t="n">
-        <v>0.1445846796115259</v>
+        <v>0.1442528979462496</v>
       </c>
       <c r="D130" t="n">
         <v>0.1796233743180209</v>
@@ -2667,7 +2667,7 @@
         <v>0.8258158877845915</v>
       </c>
       <c r="C131" t="n">
-        <v>0.1413147915004033</v>
+        <v>0.1409905133197679</v>
       </c>
       <c r="D131" t="n">
         <v>0.1714667907151423</v>
@@ -2684,7 +2684,7 @@
         <v>0.8234686684993304</v>
       </c>
       <c r="C132" t="n">
-        <v>0.1401874830409457</v>
+        <v>0.1398657917199897</v>
       </c>
       <c r="D132" t="n">
         <v>0.180577605060539</v>
@@ -2701,7 +2701,7 @@
         <v>0.8211214492140693</v>
       </c>
       <c r="C133" t="n">
-        <v>0.1332811365538554</v>
+        <v>0.1329752933790835</v>
       </c>
       <c r="D133" t="n">
         <v>0.1799977337596841</v>
@@ -2718,7 +2718,7 @@
         <v>0.8261313174032564</v>
       </c>
       <c r="C134" t="n">
-        <v>0.1360679563066724</v>
+        <v>0.1357557181549161</v>
       </c>
       <c r="D134" t="n">
         <v>0.185079534910508</v>
@@ -2735,7 +2735,7 @@
         <v>0.8311411855924438</v>
       </c>
       <c r="C135" t="n">
-        <v>0.145354365893787</v>
+        <v>0.1450208180123586</v>
       </c>
       <c r="D135" t="n">
         <v>0.1751808267042082</v>
@@ -2752,7 +2752,7 @@
         <v>0.8351272291534503</v>
       </c>
       <c r="C136" t="n">
-        <v>0.1585626661152351</v>
+        <v>0.1581988088548689</v>
       </c>
       <c r="D136" t="n">
         <v>0.1760210838161876</v>
@@ -2769,7 +2769,7 @@
         <v>0.8391132727144569</v>
       </c>
       <c r="C137" t="n">
-        <v>0.1534476979293544</v>
+        <v>0.1530955780997251</v>
       </c>
       <c r="D137" t="n">
         <v>0.1747082363812004</v>
@@ -2786,7 +2786,7 @@
         <v>0.8385687601325156</v>
       </c>
       <c r="C138" t="n">
-        <v>0.1557296267265709</v>
+        <v>0.1553722705044107</v>
       </c>
       <c r="D138" t="n">
         <v>0.17911470965871</v>
@@ -2803,7 +2803,7 @@
         <v>0.8380242475505745</v>
       </c>
       <c r="C139" t="n">
-        <v>0.1479551461218516</v>
+        <v>0.147615630172455</v>
       </c>
       <c r="D139" t="n">
         <v>0.18997063684651</v>
@@ -2820,7 +2820,7 @@
         <v>0.8402322548812292</v>
       </c>
       <c r="C140" t="n">
-        <v>0.1364265646005264</v>
+        <v>0.136113503542379</v>
       </c>
       <c r="D140" t="n">
         <v>0.1811403919759236</v>
@@ -2837,7 +2837,7 @@
         <v>0.8424402622118841</v>
       </c>
       <c r="C141" t="n">
-        <v>0.1463249152840182</v>
+        <v>0.1459891402614169</v>
       </c>
       <c r="D141" t="n">
         <v>0.1953847737141997</v>
@@ -2854,7 +2854,7 @@
         <v>0.846850990343272</v>
       </c>
       <c r="C142" t="n">
-        <v>0.1491761849965978</v>
+        <v>0.1488338671022626</v>
       </c>
       <c r="D142" t="n">
         <v>0.1986181771267929</v>
@@ -2871,7 +2871,7 @@
         <v>0.8512617184746599</v>
       </c>
       <c r="C143" t="n">
-        <v>0.1571079693794325</v>
+        <v>0.1567474502438717</v>
       </c>
       <c r="D143" t="n">
         <v>0.1670461585595581</v>
@@ -2888,7 +2888,7 @@
         <v>0.8445090575879326</v>
       </c>
       <c r="C144" t="n">
-        <v>0.1382933657734506</v>
+        <v>0.1379760209253223</v>
       </c>
       <c r="D144" t="n">
         <v>0.1761970444994387</v>
@@ -2905,7 +2905,7 @@
         <v>0.8377563967012054</v>
       </c>
       <c r="C145" t="n">
-        <v>0.1299184350350224</v>
+        <v>0.1296203083258729</v>
       </c>
       <c r="D145" t="n">
         <v>0.1848986180349593</v>
@@ -2922,7 +2922,7 @@
         <v>0.8439892154789596</v>
       </c>
       <c r="C146" t="n">
-        <v>0.1307362676872389</v>
+        <v>0.1304362642793963</v>
       </c>
       <c r="D146" t="n">
         <v>0.1914716409122512</v>
@@ -2939,7 +2939,7 @@
         <v>0.8502220342567138</v>
       </c>
       <c r="C147" t="n">
-        <v>0.1456207849379461</v>
+        <v>0.1452866256988388</v>
       </c>
       <c r="D147" t="n">
         <v>0.1800706095953441</v>
@@ -2956,7 +2956,7 @@
         <v>0.8504986959892858</v>
       </c>
       <c r="C148" t="n">
-        <v>0.1478661879119263</v>
+        <v>0.1475268760969034</v>
       </c>
       <c r="D148" t="n">
         <v>0.1793065653353114</v>
@@ -2973,7 +2973,7 @@
         <v>0.850775357721858</v>
       </c>
       <c r="C149" t="n">
-        <v>0.1421409293327644</v>
+        <v>0.1418147553953551</v>
       </c>
       <c r="D149" t="n">
         <v>0.1796008765570694</v>
@@ -2990,7 +2990,7 @@
         <v>0.851704024811447</v>
       </c>
       <c r="C150" t="n">
-        <v>0.1426904141105881</v>
+        <v>0.1423629792582941</v>
       </c>
       <c r="D150" t="n">
         <v>0.1869193937826515</v>
@@ -3007,7 +3007,7 @@
         <v>0.8526326919010361</v>
       </c>
       <c r="C151" t="n">
-        <v>0.1424998139927085</v>
+        <v>0.1421728165147247</v>
       </c>
       <c r="D151" t="n">
         <v>0.2009071451600903</v>
@@ -3024,7 +3024,7 @@
         <v>0.8527049411433002</v>
       </c>
       <c r="C152" t="n">
-        <v>0.1426988330064704</v>
+        <v>0.1423713788351496</v>
       </c>
       <c r="D152" t="n">
         <v>0.1973719065991862</v>
@@ -3041,7 +3041,7 @@
         <v>0.8527771903855643</v>
       </c>
       <c r="C153" t="n">
-        <v>0.1378671959399422</v>
+        <v>0.137550829033166</v>
       </c>
       <c r="D153" t="n">
         <v>0.1913747246525353</v>
@@ -3058,7 +3058,7 @@
         <v>0.8539508000281948</v>
       </c>
       <c r="C154" t="n">
-        <v>0.1401368790755262</v>
+        <v>0.13981530387661</v>
       </c>
       <c r="D154" t="n">
         <v>0.1989575980189847</v>
@@ -3075,7 +3075,7 @@
         <v>0.8551244096708254</v>
       </c>
       <c r="C155" t="n">
-        <v>0.1343313308577151</v>
+        <v>0.1340230777788239</v>
       </c>
       <c r="D155" t="n">
         <v>0.1893291761631765</v>
@@ -3092,7 +3092,7 @@
         <v>0.8531736801296962</v>
       </c>
       <c r="C156" t="n">
-        <v>0.128027859442869</v>
+        <v>0.1277340710793864</v>
       </c>
       <c r="D156" t="n">
         <v>0.1937471863582005</v>
@@ -3109,7 +3109,7 @@
         <v>0.851222950588567</v>
       </c>
       <c r="C157" t="n">
-        <v>0.1283565015774699</v>
+        <v>0.1280619590716052</v>
       </c>
       <c r="D157" t="n">
         <v>0.1905493735664069</v>
@@ -3126,7 +3126,7 @@
         <v>0.8556477761330795</v>
       </c>
       <c r="C158" t="n">
-        <v>0.1285341972102487</v>
+        <v>0.1282392469422815</v>
       </c>
       <c r="D158" t="n">
         <v>0.1936544506068213</v>
@@ -3143,7 +3143,7 @@
         <v>0.8600726016775921</v>
       </c>
       <c r="C159" t="n">
-        <v>0.129965772403365</v>
+        <v>0.1296675370681084</v>
       </c>
       <c r="D159" t="n">
         <v>0.187309768600663</v>
@@ -3160,7 +3160,7 @@
         <v>0.8633555367590047</v>
       </c>
       <c r="C160" t="n">
-        <v>0.1384365940927099</v>
+        <v>0.1381189205753865</v>
       </c>
       <c r="D160" t="n">
         <v>0.1837018392160625</v>
@@ -3177,7 +3177,7 @@
         <v>0.8666384718404173</v>
       </c>
       <c r="C161" t="n">
-        <v>0.1457355103700691</v>
+        <v>0.1454010878679728</v>
       </c>
       <c r="D161" t="n">
         <v>0.1167730296868646</v>
@@ -3194,7 +3194,7 @@
         <v>0.8689786424191162</v>
       </c>
       <c r="C162" t="n">
-        <v>0.1456882756606804</v>
+        <v>0.1453539615491174</v>
       </c>
       <c r="D162" t="n">
         <v>0.1894177738842653</v>
@@ -3211,7 +3211,7 @@
         <v>0.8713188129978149</v>
       </c>
       <c r="C163" t="n">
-        <v>0.1433344467455143</v>
+        <v>0.1430055340172746</v>
       </c>
       <c r="D163" t="n">
         <v>0.1939588557930332</v>
@@ -3228,7 +3228,7 @@
         <v>0.871373440473673</v>
       </c>
       <c r="C164" t="n">
-        <v>0.1415007553282493</v>
+        <v>0.141176050412301</v>
       </c>
       <c r="D164" t="n">
         <v>0.2023242754612356</v>
@@ -3245,7 +3245,7 @@
         <v>0.8714280679495312</v>
       </c>
       <c r="C165" t="n">
-        <v>0.1363623738670786</v>
+        <v>0.1360494601088284</v>
       </c>
       <c r="D165" t="n">
         <v>0.2073607755430541</v>
@@ -3262,7 +3262,7 @@
         <v>0.8718192711637415</v>
       </c>
       <c r="C166" t="n">
-        <v>0.1314836730403848</v>
+        <v>0.1311819545449315</v>
       </c>
       <c r="D166" t="n">
         <v>0.2061207017827546</v>
@@ -3279,7 +3279,7 @@
         <v>0.8722104743779516</v>
       </c>
       <c r="C167" t="n">
-        <v>0.1233073932948388</v>
+        <v>0.1230244370895329</v>
       </c>
       <c r="D167" t="n">
         <v>0.153059386377136</v>
@@ -3296,7 +3296,7 @@
         <v>0.8675072249242264</v>
       </c>
       <c r="C168" t="n">
-        <v>0.1118376852809201</v>
+        <v>0.1115810488685225</v>
       </c>
       <c r="D168" t="n">
         <v>0.1959637857942323</v>
@@ -3313,7 +3313,7 @@
         <v>0.8628039754705011</v>
       </c>
       <c r="C169" t="n">
-        <v>0.1013903534140483</v>
+        <v>0.10115769072538</v>
       </c>
       <c r="D169" t="n">
         <v>0.1973797117788344</v>
@@ -3330,7 +3330,7 @@
         <v>0.8652815958271657</v>
       </c>
       <c r="C170" t="n">
-        <v>0.09000538134126225</v>
+        <v>0.08979884400006212</v>
       </c>
       <c r="D170" t="n">
         <v>0.2010906054619881</v>
@@ -3347,7 +3347,7 @@
         <v>0.8677592161838302</v>
       </c>
       <c r="C171" t="n">
-        <v>0.095279886929469</v>
+        <v>0.09506124606352291</v>
       </c>
       <c r="D171" t="n">
         <v>0.197404990699299</v>
@@ -3364,7 +3364,7 @@
         <v>0.8720219214774089</v>
       </c>
       <c r="C172" t="n">
-        <v>0.1165567028725586</v>
+        <v>0.1162892376260188</v>
       </c>
       <c r="D172" t="n">
         <v>0.1950639035677117</v>
@@ -3381,7 +3381,7 @@
         <v>0.8762846267709875</v>
       </c>
       <c r="C173" t="n">
-        <v>0.1116418079368718</v>
+        <v>0.1113856210085522</v>
       </c>
       <c r="D173" t="n">
         <v>0.1420771244826796</v>
@@ -3398,7 +3398,7 @@
         <v>0.8793983928949037</v>
       </c>
       <c r="C174" t="n">
-        <v>0.1297705350862955</v>
+        <v>0.1294727477664327</v>
       </c>
       <c r="D174" t="n">
         <v>0.1968391134195387</v>
@@ -3415,7 +3415,7 @@
         <v>0.88251215901882</v>
       </c>
       <c r="C175" t="n">
-        <v>0.1222419418220156</v>
+        <v>0.1219614305317925</v>
       </c>
       <c r="D175" t="n">
         <v>0.1947848516796856</v>
@@ -3432,7 +3432,7 @@
         <v>0.8840082469866779</v>
       </c>
       <c r="C176" t="n">
-        <v>0.1293653089660864</v>
+        <v>0.129068451527573</v>
       </c>
       <c r="D176" t="n">
         <v>0.2031655254486631</v>
@@ -3449,7 +3449,7 @@
         <v>0.8855043349545357</v>
       </c>
       <c r="C177" t="n">
-        <v>0.1217611204642333</v>
+        <v>0.1214817125254248</v>
       </c>
       <c r="D177" t="n">
         <v>0.205532590655634</v>
@@ -3466,7 +3466,7 @@
         <v>0.8855078593078169</v>
       </c>
       <c r="C178" t="n">
-        <v>0.1075653919937593</v>
+        <v>0.1073185593073524</v>
       </c>
       <c r="D178" t="n">
         <v>0.2072257158094996</v>
@@ -3483,7 +3483,7 @@
         <v>0.8855113836610982</v>
       </c>
       <c r="C179" t="n">
-        <v>0.09977285626156693</v>
+        <v>0.09954390527942426</v>
       </c>
       <c r="D179" t="n">
         <v>0.1689419275238304</v>
@@ -3500,7 +3500,7 @@
         <v>0.8845527595686191</v>
       </c>
       <c r="C180" t="n">
-        <v>0.09560763796751173</v>
+        <v>0.09538824500400254</v>
       </c>
       <c r="D180" t="n">
         <v>0.1959182175685206</v>
@@ -3517,7 +3517,7 @@
         <v>0.8835941354761402</v>
       </c>
       <c r="C181" t="n">
-        <v>0.09425141776786816</v>
+        <v>0.09403513695287656</v>
       </c>
       <c r="D181" t="n">
         <v>0.1956780755531269</v>
@@ -3534,7 +3534,7 @@
         <v>0.8870092338055967</v>
       </c>
       <c r="C182" t="n">
-        <v>0.0954781492371265</v>
+        <v>0.09525905341427368</v>
       </c>
       <c r="D182" t="n">
         <v>0.2003361331849968</v>
@@ -3551,7 +3551,7 @@
         <v>0.8904243321350532</v>
       </c>
       <c r="C183" t="n">
-        <v>0.08345459273537595</v>
+        <v>0.08326308763381818</v>
       </c>
       <c r="D183" t="n">
         <v>0.1985570178389782</v>
@@ -3568,7 +3568,7 @@
         <v>0.8930411644463241</v>
       </c>
       <c r="C184" t="n">
-        <v>0.08999585147883807</v>
+        <v>0.08978933600602422</v>
       </c>
       <c r="D184" t="n">
         <v>0.1976392657212258</v>
@@ -3585,7 +3585,7 @@
         <v>0.8956579967575949</v>
       </c>
       <c r="C185" t="n">
-        <v>0.09452268645675116</v>
+        <v>0.09430578315549354</v>
       </c>
       <c r="D185" t="n">
         <v>0.1383340521142389</v>
@@ -3602,7 +3602,7 @@
         <v>0.8981990554733206</v>
       </c>
       <c r="C186" t="n">
-        <v>0.0953574817052834</v>
+        <v>0.09513866278088737</v>
       </c>
       <c r="D186" t="n">
         <v>0.1971723293637559</v>
@@ -3619,7 +3619,7 @@
         <v>0.9007401141890462</v>
       </c>
       <c r="C187" t="n">
-        <v>0.09758641656493569</v>
+        <v>0.09736248285437066</v>
       </c>
       <c r="D187" t="n">
         <v>0.2008348436472908</v>
@@ -3636,7 +3636,7 @@
         <v>0.9016582082187918</v>
       </c>
       <c r="C188" t="n">
-        <v>0.09685488270829221</v>
+        <v>0.09663262766466349</v>
       </c>
       <c r="D188" t="n">
         <v>0.2048448051783072</v>
@@ -3653,7 +3653,7 @@
         <v>0.9025763022485372</v>
       </c>
       <c r="C189" t="n">
-        <v>0.09123882357075641</v>
+        <v>0.09102945582236499</v>
       </c>
       <c r="D189" t="n">
         <v>0.2090681968160502</v>
@@ -3670,7 +3670,7 @@
         <v>0.9056407274265172</v>
       </c>
       <c r="C190" t="n">
-        <v>0.09285138957801892</v>
+        <v>0.0926383214387099</v>
       </c>
       <c r="D190" t="n">
         <v>0.2011835317054947</v>
@@ -3687,7 +3687,7 @@
         <v>0.9087051526044971</v>
       </c>
       <c r="C191" t="n">
-        <v>0.09448609348578166</v>
+        <v>0.09426927415522465</v>
       </c>
       <c r="D191" t="n">
         <v>0.1532950480150173</v>
@@ -3704,7 +3704,7 @@
         <v>0.9071491506308592</v>
       </c>
       <c r="C192" t="n">
-        <v>0.09220093514041675</v>
+        <v>0.09198935961330616</v>
       </c>
       <c r="D192" t="n">
         <v>0.1976521720549584</v>
@@ -3721,7 +3721,7 @@
         <v>0.9055931486572213</v>
       </c>
       <c r="C193" t="n">
-        <v>0.09070298303580811</v>
+        <v>0.09049484489255526</v>
       </c>
       <c r="D193" t="n">
         <v>0.2005315524629018</v>
@@ -3738,7 +3738,7 @@
         <v>0.9111581024881933</v>
       </c>
       <c r="C194" t="n">
-        <v>0.09377077344390637</v>
+        <v>0.09355559557408598</v>
       </c>
       <c r="D194" t="n">
         <v>0.201611552921882</v>
@@ -3755,7 +3755,7 @@
         <v>0.9167230563191654</v>
       </c>
       <c r="C195" t="n">
-        <v>0.09640861478368851</v>
+        <v>0.09618738380094635</v>
       </c>
       <c r="D195" t="n">
         <v>0.2072599774711565</v>
@@ -3772,7 +3772,7 @@
         <v>0.9197874814971453</v>
       </c>
       <c r="C196" t="n">
-        <v>0.09977304741158821</v>
+        <v>0.09954409599080938</v>
       </c>
       <c r="D196" t="n">
         <v>0.2085264301355848</v>
@@ -3789,7 +3789,7 @@
         <v>0.9228519066751252</v>
       </c>
       <c r="C197" t="n">
-        <v>0.09970180408630895</v>
+        <v>0.09947301614916589</v>
       </c>
       <c r="D197" t="n">
         <v>0.1530039641015849</v>
@@ -3806,7 +3806,7 @@
         <v>0.9236202156904207</v>
       </c>
       <c r="C198" t="n">
-        <v>0.1007232176381703</v>
+        <v>0.1004920858407366</v>
       </c>
       <c r="D198" t="n">
         <v>0.195534914602317</v>
@@ -3823,7 +3823,7 @@
         <v>0.9243885247057165</v>
       </c>
       <c r="C199" t="n">
-        <v>0.09995796954469548</v>
+        <v>0.0997285937790038</v>
       </c>
       <c r="D199" t="n">
         <v>0.2068394348154305</v>
@@ -3840,7 +3840,7 @@
         <v>0.9264802283780926</v>
       </c>
       <c r="C200" t="n">
-        <v>0.09730374943652889</v>
+        <v>0.0970804643684814</v>
       </c>
       <c r="D200" t="n">
         <v>0.1998963327303955</v>
@@ -3857,7 +3857,7 @@
         <v>0.9285719320504687</v>
       </c>
       <c r="C201" t="n">
-        <v>0.09928148463030366</v>
+        <v>0.09905366120952178</v>
       </c>
       <c r="D201" t="n">
         <v>0.206338349660117</v>
@@ -3874,7 +3874,7 @@
         <v>0.932094523155001</v>
       </c>
       <c r="C202" t="n">
-        <v>0.1036375577801095</v>
+        <v>0.1033997383818313</v>
       </c>
       <c r="D202" t="n">
         <v>0.2073824008167201</v>
@@ -3891,7 +3891,7 @@
         <v>0.9356171142595333</v>
       </c>
       <c r="C203" t="n">
-        <v>0.1005860181111379</v>
+        <v>0.1003552011484964</v>
       </c>
       <c r="D203" t="n">
         <v>0.1678036855110897</v>
@@ -3908,7 +3908,7 @@
         <v>0.935934306054839</v>
       </c>
       <c r="C204" t="n">
-        <v>0.1055843336019461</v>
+        <v>0.1053420468940897</v>
       </c>
       <c r="D204" t="n">
         <v>0.199907193047198</v>
@@ -3925,7 +3925,7 @@
         <v>0.9362514978501444</v>
       </c>
       <c r="C205" t="n">
-        <v>0.1021199968379685</v>
+        <v>0.1018856598203816</v>
       </c>
       <c r="D205" t="n">
         <v>0.1988781864996311</v>
@@ -3942,7 +3942,7 @@
         <v>0.9425865228730528</v>
       </c>
       <c r="C206" t="n">
-        <v>0.1040434990530923</v>
+        <v>0.1038047481323878</v>
       </c>
       <c r="D206" t="n">
         <v>0.2026339178050436</v>
@@ -3959,7 +3959,7 @@
         <v>0.9489215478959611</v>
       </c>
       <c r="C207" t="n">
-        <v>0.1080595126408094</v>
+        <v>0.1078115460848143</v>
       </c>
       <c r="D207" t="n">
         <v>0.2012811284805402</v>
@@ -3976,7 +3976,7 @@
         <v>0.9523807006414322</v>
       </c>
       <c r="C208" t="n">
-        <v>0.109494028942173</v>
+        <v>0.1092427705698623</v>
       </c>
       <c r="D208" t="n">
         <v>0.1936200511789097</v>
@@ -3993,7 +3993,7 @@
         <v>0.9558398533869034</v>
       </c>
       <c r="C209" t="n">
-        <v>0.1135232012093949</v>
+        <v>0.1132626970062805</v>
       </c>
       <c r="D209" t="n">
         <v>0.1677059179233804</v>
@@ -4010,7 +4010,7 @@
         <v>0.9580460985409177</v>
       </c>
       <c r="C210" t="n">
-        <v>0.1155476758045292</v>
+        <v>0.1152825259947413</v>
       </c>
       <c r="D210" t="n">
         <v>0.1967546241115967</v>
@@ -4027,7 +4027,7 @@
         <v>0.960252343694932</v>
       </c>
       <c r="C211" t="n">
-        <v>0.1147510867570524</v>
+        <v>0.1144877648977875</v>
       </c>
       <c r="D211" t="n">
         <v>0.2062999390740727</v>
@@ -4044,7 +4044,7 @@
         <v>0.9626876718122225</v>
       </c>
       <c r="C212" t="n">
-        <v>0.1123417315570395</v>
+        <v>0.1120839384984929</v>
       </c>
       <c r="D212" t="n">
         <v>0.2034927897551921</v>
@@ -4061,7 +4061,7 @@
         <v>0.9651229999295129</v>
       </c>
       <c r="C213" t="n">
-        <v>0.1105351338718394</v>
+        <v>0.1102814864529976</v>
       </c>
       <c r="D213" t="n">
         <v>0.2056732665313098</v>
@@ -4078,7 +4078,7 @@
         <v>0.9683689293014731</v>
       </c>
       <c r="C214" t="n">
-        <v>0.1111559827488945</v>
+        <v>0.1109009106543894</v>
       </c>
       <c r="D214" t="n">
         <v>0.199407471839572</v>
@@ -4095,7 +4095,7 @@
         <v>0.9716148586734333</v>
       </c>
       <c r="C215" t="n">
-        <v>0.1160953838787606</v>
+        <v>0.115828977231129</v>
       </c>
       <c r="D215" t="n">
         <v>0.1611749744274283</v>
@@ -4112,7 +4112,7 @@
         <v>0.9702685557200252</v>
       </c>
       <c r="C216" t="n">
-        <v>0.1122988056838986</v>
+        <v>0.1120411111283035</v>
       </c>
       <c r="D216" t="n">
         <v>0.2010783497515474</v>
@@ -4129,7 +4129,7 @@
         <v>0.9689222527666174</v>
       </c>
       <c r="C217" t="n">
-        <v>0.1042808127396134</v>
+        <v>0.1040415172499386</v>
       </c>
       <c r="D217" t="n">
         <v>0.2007385003746517</v>
@@ -4146,7 +4146,7 @@
         <v>0.9719761048847536</v>
       </c>
       <c r="C218" t="n">
-        <v>0.09975553875524179</v>
+        <v>0.0995266275119643</v>
       </c>
       <c r="D218" t="n">
         <v>0.1883791166056598</v>
@@ -4163,7 +4163,7 @@
         <v>0.9750299570028899</v>
       </c>
       <c r="C219" t="n">
-        <v>0.0995661715855488</v>
+        <v>0.09933769488730801</v>
       </c>
       <c r="D219" t="n">
         <v>0.2029681227521643</v>
@@ -4180,7 +4180,7 @@
         <v>0.9814090364418128</v>
       </c>
       <c r="C220" t="n">
-        <v>0.102159238683497</v>
+        <v>0.1019248116167785</v>
       </c>
       <c r="D220" t="n">
         <v>0.1962484477402905</v>
@@ -4197,7 +4197,7 @@
         <v>0.9877881158807358</v>
       </c>
       <c r="C221" t="n">
-        <v>0.1182642290607439</v>
+        <v>0.117992845516057</v>
       </c>
       <c r="D221" t="n">
         <v>0.181921605565962</v>
@@ -4214,7 +4214,7 @@
         <v>0.9889881581729753</v>
       </c>
       <c r="C222" t="n">
-        <v>0.1219124809570391</v>
+        <v>0.1216327256879568</v>
       </c>
       <c r="D222" t="n">
         <v>0.1902955039903355</v>
@@ -4231,7 +4231,7 @@
         <v>0.9901882004652146</v>
       </c>
       <c r="C223" t="n">
-        <v>0.1147357643189681</v>
+        <v>0.1144724776204411</v>
       </c>
       <c r="D223" t="n">
         <v>0.2097581044718746</v>
@@ -4248,7 +4248,7 @@
         <v>0.9907009938676252</v>
       </c>
       <c r="C224" t="n">
-        <v>0.1110728672739206</v>
+        <v>0.1108179859063361</v>
       </c>
       <c r="D224" t="n">
         <v>0.2006659943116632</v>
@@ -4265,7 +4265,7 @@
         <v>0.991213787270036</v>
       </c>
       <c r="C225" t="n">
-        <v>0.107595355683794</v>
+        <v>0.1073484542390442</v>
       </c>
       <c r="D225" t="n">
         <v>0.1995533179020576</v>
@@ -4282,7 +4282,7 @@
         <v>0.9958906040741524</v>
       </c>
       <c r="C226" t="n">
-        <v>0.111066415876903</v>
+        <v>0.110811549313482</v>
       </c>
       <c r="D226" t="n">
         <v>0.2073520918414291</v>
@@ -4299,7 +4299,7 @@
         <v>1.000567420878269</v>
       </c>
       <c r="C227" t="n">
-        <v>0.1234099746038231</v>
+        <v>0.1231267830029164</v>
       </c>
       <c r="D227" t="n">
         <v>0.148915502234934</v>
@@ -4316,7 +4316,7 @@
         <v>0.9982642560090224</v>
       </c>
       <c r="C228" t="n">
-        <v>0.1185257303241864</v>
+        <v>0.1182537467067609</v>
       </c>
       <c r="D228" t="n">
         <v>0.2014496650455873</v>
@@ -4333,7 +4333,7 @@
         <v>0.9959610911397758</v>
       </c>
       <c r="C229" t="n">
-        <v>0.108739187668528</v>
+        <v>0.1084896614471994</v>
       </c>
       <c r="D229" t="n">
         <v>0.1922765876133251</v>
@@ -4350,7 +4350,7 @@
         <v>1</v>
       </c>
       <c r="C230" t="n">
-        <v>0.10467</v>
+        <v>0.1044298114337025</v>
       </c>
       <c r="D230" t="n">
         <v>0.1991</v>
@@ -4367,7 +4367,7 @@
         <v>1.004038908860224</v>
       </c>
       <c r="C231" t="n">
-        <v>0.10299401655399</v>
+        <v>0.1027576739040108</v>
       </c>
       <c r="D231" t="n">
         <v>0.215828289210421</v>
@@ -4384,7 +4384,7 @@
         <v>1.000726016775922</v>
       </c>
       <c r="C232" t="n">
-        <v>0.09778900354292716</v>
+        <v>0.09756460495153864</v>
       </c>
       <c r="D232" t="n">
         <v>0.2031525078712149</v>
@@ -4401,7 +4401,7 @@
         <v>0.9974131246916189</v>
       </c>
       <c r="C233" t="n">
-        <v>0.0850299619089348</v>
+        <v>0.08483484177285724</v>
       </c>
       <c r="D233" t="n">
         <v>0.2048298693313923</v>
@@ -4418,7 +4418,7 @@
         <v>1.000636145767251</v>
       </c>
       <c r="C234" t="n">
-        <v>0.08307715082214917</v>
+        <v>0.08288651184490591</v>
       </c>
       <c r="D234" t="n">
         <v>0.1859816885360515</v>
@@ -4435,7 +4435,7 @@
         <v>1.003859166842884</v>
       </c>
       <c r="C235" t="n">
-        <v>0.08881723945442098</v>
+        <v>0.08861342856871296</v>
       </c>
       <c r="D235" t="n">
         <v>0.196342282374006</v>
@@ -4452,7 +4452,7 @@
         <v>1.006595827165715</v>
       </c>
       <c r="C236" t="n">
-        <v>0.09245021436461767</v>
+        <v>0.09223806681095249</v>
       </c>
       <c r="D236" t="n">
         <v>0.1989875127577146</v>
@@ -4469,7 +4469,7 @@
         <v>1.009332487488546</v>
       </c>
       <c r="C237" t="n">
-        <v>0.09380457002388369</v>
+        <v>0.09358931460030301</v>
       </c>
       <c r="D237" t="n">
         <v>0.2049869617442072</v>
@@ -4486,7 +4486,7 @@
         <v>1.010134277860013</v>
       </c>
       <c r="C238" t="n">
-        <v>0.09426469538458317</v>
+        <v>0.09404838410115055</v>
       </c>
       <c r="D238" t="n">
         <v>0.2094771008546293</v>
@@ -4503,7 +4503,7 @@
         <v>1.01093606823148</v>
       </c>
       <c r="C239" t="n">
-        <v>0.09309194019027829</v>
+        <v>0.09287832005415375</v>
       </c>
       <c r="D239" t="n">
         <v>0.2055520685531806</v>
@@ -4520,7 +4520,7 @@
         <v>1.011859448791147</v>
       </c>
       <c r="C240" t="n">
-        <v>0.09235472388150678</v>
+        <v>0.09214279545196727</v>
       </c>
       <c r="D240" t="n">
         <v>0.2193980599432264</v>
@@ -4537,7 +4537,7 @@
         <v>1.012782829350814</v>
       </c>
       <c r="C241" t="n">
-        <v>0.09309991961498709</v>
+        <v>0.09288628116830003</v>
       </c>
       <c r="D241" t="n">
         <v>0.2016226915407824</v>
@@ -4554,7 +4554,7 @@
         <v>1.016774159441743</v>
       </c>
       <c r="C242" t="n">
-        <v>0.09624556160409289</v>
+        <v>0.09602470478309179</v>
       </c>
       <c r="D242" t="n">
         <v>0.2109613014927235</v>
@@ -4571,7 +4571,7 @@
         <v>1.020765489532671</v>
       </c>
       <c r="C243" t="n">
-        <v>0.100924258369241</v>
+        <v>0.1006926652391908</v>
       </c>
       <c r="D243" t="n">
         <v>0.2204228123964203</v>
@@ -4588,7 +4588,7 @@
         <v>1.028945513498273</v>
       </c>
       <c r="C244" t="n">
-        <v>0.1102390734125013</v>
+        <v>0.10998610537015</v>
       </c>
       <c r="D244" t="n">
         <v>0.214199874637356</v>
@@ -4605,7 +4605,7 @@
         <v>1.037125537463875</v>
       </c>
       <c r="C245" t="n">
-        <v>0.1131299883781782</v>
+        <v>0.1128703864892529</v>
       </c>
       <c r="D245" t="n">
         <v>0.2253343414640777</v>
@@ -4622,7 +4622,7 @@
         <v>1.042716923944456</v>
       </c>
       <c r="C246" t="n">
-        <v>0.1170403943750517</v>
+        <v>0.1167718191909127</v>
       </c>
       <c r="D246" t="n">
         <v>0.2180841173458437</v>
@@ -4639,7 +4639,7 @@
         <v>1.048308310425037</v>
       </c>
       <c r="C247" t="n">
-        <v>0.1196785323099577</v>
+        <v>0.1194039033322935</v>
       </c>
       <c r="D247" t="n">
         <v>0.2206411965829207</v>
@@ -4656,7 +4656,7 @@
         <v>1.052481144709946</v>
       </c>
       <c r="C248" t="n">
-        <v>0.1212278249746343</v>
+        <v>0.1209496408007925</v>
       </c>
       <c r="D248" t="n">
         <v>0.213685538339958</v>
@@ -4673,7 +4673,7 @@
         <v>1.056653978994854</v>
       </c>
       <c r="C249" t="n">
-        <v>0.1226229234694728</v>
+        <v>0.1223415379322287</v>
       </c>
       <c r="D249" t="n">
         <v>0.2213591247936227</v>
@@ -4690,7 +4690,7 @@
         <v>1.061901741030521</v>
       </c>
       <c r="C250" t="n">
-        <v>0.121762678225314</v>
+        <v>0.1214832667118767</v>
       </c>
       <c r="D250" t="n">
         <v>0.2212069073095611</v>
@@ -4707,7 +4707,7 @@
         <v>1.067149503066187</v>
       </c>
       <c r="C251" t="n">
-        <v>0.1236940087782743</v>
+        <v>0.1234101653978592</v>
       </c>
       <c r="D251" t="n">
         <v>0.2063440964619394</v>
@@ -4724,7 +4724,7 @@
         <v>1.072992880806372</v>
       </c>
       <c r="C252" t="n">
-        <v>0.1285563049554772</v>
+        <v>0.1282613039563776</v>
       </c>
       <c r="D252" t="n">
         <v>0.2224618674269423</v>
@@ -4741,7 +4741,7 @@
         <v>1.078836258546557</v>
       </c>
       <c r="C253" t="n">
-        <v>0.1278321885341496</v>
+        <v>0.1275388491810333</v>
       </c>
       <c r="D253" t="n">
         <v>0.2167150002123427</v>
@@ -4758,7 +4758,7 @@
         <v>1.087540373782951</v>
       </c>
       <c r="C254" t="n">
-        <v>0.1264504778996333</v>
+        <v>0.1261603091884997</v>
       </c>
       <c r="D254" t="n">
         <v>0.2121300556387827</v>
@@ -4775,7 +4775,7 @@
         <v>1.096244489019346</v>
       </c>
       <c r="C255" t="n">
-        <v>0.1275262967342798</v>
+        <v>0.1272336593178487</v>
       </c>
       <c r="D255" t="n">
         <v>0.2311528153967561</v>
@@ -4792,7 +4792,7 @@
         <v>1.106462653781992</v>
       </c>
       <c r="C256" t="n">
-        <v>0.1533264583491549</v>
+        <v>0.1529746167306744</v>
       </c>
       <c r="D256" t="n">
         <v>0.2383270678848933</v>
@@ -4809,7 +4809,7 @@
         <v>1.116680818544638</v>
       </c>
       <c r="C257" t="n">
-        <v>0.1529174650125631</v>
+        <v>0.1525665619201468</v>
       </c>
       <c r="D257" t="n">
         <v>0.2084749698695519</v>
@@ -4826,7 +4826,7 @@
         <v>1.125836878606931</v>
       </c>
       <c r="C258" t="n">
-        <v>0.156443622825659</v>
+        <v>0.1560846281808431</v>
       </c>
       <c r="D258" t="n">
         <v>0.2416868777088617</v>
@@ -4843,7 +4843,7 @@
         <v>1.134992938669225</v>
       </c>
       <c r="C259" t="n">
-        <v>0.1663622684925166</v>
+        <v>0.1659805133118992</v>
       </c>
       <c r="D259" t="n">
         <v>0.248107270455951</v>
@@ -4860,7 +4860,7 @@
         <v>1.135402138707049</v>
       </c>
       <c r="C260" t="n">
-        <v>0.1558126358661418</v>
+        <v>0.1554550891610714</v>
       </c>
       <c r="D260" t="n">
         <v>0.230579097110146</v>
@@ -4877,7 +4877,7 @@
         <v>1.135811338744872</v>
       </c>
       <c r="C261" t="n">
-        <v>0.1408596608806502</v>
+        <v>0.1405364270983241</v>
       </c>
       <c r="D261" t="n">
         <v>0.2332253526300659</v>
@@ -4894,7 +4894,7 @@
         <v>1.140294553096823</v>
       </c>
       <c r="C262" t="n">
-        <v>0.141410830703414</v>
+        <v>0.1410863321394932</v>
       </c>
       <c r="D262" t="n">
         <v>0.2276604753525971</v>
@@ -4911,7 +4911,7 @@
         <v>1.144777767448774</v>
       </c>
       <c r="C263" t="n">
-        <v>0.1547461918262026</v>
+        <v>0.1543910923138807</v>
       </c>
       <c r="D263" t="n">
         <v>0.2250218403298324</v>
@@ -4928,7 +4928,7 @@
         <v>1.141831939302186</v>
       </c>
       <c r="C264" t="n">
-        <v>0.1359131713331141</v>
+        <v>0.1356012883698635</v>
       </c>
       <c r="D264" t="n">
         <v>0.2235004918113972</v>
@@ -4945,7 +4945,7 @@
         <v>1.138886111155598</v>
       </c>
       <c r="C265" t="n">
-        <v>0.1163768692073303</v>
+        <v>0.1161098166290834</v>
       </c>
       <c r="D265" t="n">
         <v>0.2286444600995081</v>

</xml_diff>

<commit_message>
analaysis now till 2023
</commit_message>
<xml_diff>
--- a/package/calibration_data/aligned_data.xlsx
+++ b/package/calibration_data/aligned_data.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E265"/>
+  <dimension ref="A1:E277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,13 +471,13 @@
         <v>36892</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6292944244731091</v>
+        <v>0.6337245365475435</v>
       </c>
       <c r="C2" t="n">
-        <v>0.07828877025570641</v>
+        <v>0.07774148510829536</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1730509532023567</v>
+        <v>0.1718412239382025</v>
       </c>
       <c r="E2" t="n">
         <v>0.34327</v>
@@ -4952,6 +4952,210 @@
       </c>
       <c r="E265" t="n">
         <v>0.28776</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="2" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B266" t="n">
+        <v>1.147118638814245</v>
+      </c>
+      <c r="C266" t="n">
+        <v>0.1139719076886744</v>
+      </c>
+      <c r="D266" t="n">
+        <v>0.2307520696147135</v>
+      </c>
+      <c r="E266" t="n">
+        <v>0.24903</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="2" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B267" t="n">
+        <v>1.155351166472892</v>
+      </c>
+      <c r="C267" t="n">
+        <v>0.1189369534626325</v>
+      </c>
+      <c r="D267" t="n">
+        <v>0.2358590252969582</v>
+      </c>
+      <c r="E267" t="n">
+        <v>0.23755</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="2" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B268" t="n">
+        <v>1.159280358753098</v>
+      </c>
+      <c r="C268" t="n">
+        <v>0.1235684903256264</v>
+      </c>
+      <c r="D268" t="n">
+        <v>0.2621453884777878</v>
+      </c>
+      <c r="E268" t="n">
+        <v>0.2074</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="2" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B269" t="n">
+        <v>1.163209551033304</v>
+      </c>
+      <c r="C269" t="n">
+        <v>0.1231768212583258</v>
+      </c>
+      <c r="D269" t="n">
+        <v>0.2553280272984077</v>
+      </c>
+      <c r="E269" t="n">
+        <v>0.17092</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="2" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B270" t="n">
+        <v>1.166709031091589</v>
+      </c>
+      <c r="C270" t="n">
+        <v>0.1216016047969423</v>
+      </c>
+      <c r="D270" t="n">
+        <v>0.2555907188967245</v>
+      </c>
+      <c r="E270" t="n">
+        <v>0.1307</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="2" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B271" t="n">
+        <v>1.170208511149873</v>
+      </c>
+      <c r="C271" t="n">
+        <v>0.1222866409192133</v>
+      </c>
+      <c r="D271" t="n">
+        <v>0.2669609706504602</v>
+      </c>
+      <c r="E271" t="n">
+        <v>0.14978</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="2" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B272" t="n">
+        <v>1.173719182562309</v>
+      </c>
+      <c r="C272" t="n">
+        <v>0.1229919207237912</v>
+      </c>
+      <c r="D272" t="n">
+        <v>0.2509970053968685</v>
+      </c>
+      <c r="E272" t="n">
+        <v>0.22925</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="2" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B273" t="n">
+        <v>1.177229853974744</v>
+      </c>
+      <c r="C273" t="n">
+        <v>0.1304306391350569</v>
+      </c>
+      <c r="D273" t="n">
+        <v>0.2545806997572367</v>
+      </c>
+      <c r="E273" t="n">
+        <v>0.23604</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="2" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B274" t="n">
+        <v>1.179208384935429</v>
+      </c>
+      <c r="C274" t="n">
+        <v>0.1401109389353736</v>
+      </c>
+      <c r="D274" t="n">
+        <v>0.2544927629703319</v>
+      </c>
+      <c r="E274" t="n">
+        <v>0.20583</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="2" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B275" t="n">
+        <v>1.181186915896113</v>
+      </c>
+      <c r="C275" t="n">
+        <v>0.1405350854268179</v>
+      </c>
+      <c r="D275" t="n">
+        <v>0.2690514056015423</v>
+      </c>
+      <c r="E275" t="n">
+        <v>0.24936</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="2" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B276" t="n">
+        <v>1.179856082742833</v>
+      </c>
+      <c r="C276" t="n">
+        <v>0.1251934609210341</v>
+      </c>
+      <c r="D276" t="n">
+        <v>0.2503695190631033</v>
+      </c>
+      <c r="E276" t="n">
+        <v>0.25939</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="2" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B277" t="n">
+        <v>1.178525249589552</v>
+      </c>
+      <c r="C277" t="n">
+        <v>0.1157601160791554</v>
+      </c>
+      <c r="D277" t="n">
+        <v>0.2470884693403191</v>
+      </c>
+      <c r="E277" t="n">
+        <v>0.27367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>